<commit_message>
Added all parts. Schematic finished. Consider Rev 1.0
</commit_message>
<xml_diff>
--- a/BOM_Initial.xlsx
+++ b/BOM_Initial.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\EENG393\Projects\lab06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Gilliland\Desktop\All Projects\benchBoddy\benchBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABCD03D-FCC5-4FA7-B5B1-20211BB66EC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31335" yWindow="3075" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PreBOM" sheetId="2" r:id="rId1"/>
+    <sheet name="Main Board Additions" sheetId="3" r:id="rId1"/>
+    <sheet name="MCU Board" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PreBOM!$A$1:$N$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Board Additions'!$A$1:$N$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCU Board'!$A$1:$N$33</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
   <si>
     <t>Usage</t>
   </si>
@@ -138,16 +141,148 @@
   </si>
   <si>
     <t>H11L1S(TA)</t>
+  </si>
+  <si>
+    <t>1A 3.3V Linear Reg</t>
+  </si>
+  <si>
+    <t>IC, Volt Reg</t>
+  </si>
+  <si>
+    <t>SOT223</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 1A SOT223</t>
+  </si>
+  <si>
+    <t>AP2114HA-3.3TRG1DICT-ND</t>
+  </si>
+  <si>
+    <t>Custom-Unchecked</t>
+  </si>
+  <si>
+    <t>102-5018-ND</t>
+  </si>
+  <si>
+    <t>5V 1.0A DC-DC NON-ISOLATED</t>
+  </si>
+  <si>
+    <t>3-SIP Module</t>
+  </si>
+  <si>
+    <t>DCDC Converter</t>
+  </si>
+  <si>
+    <t>5W 5V Switch Mode Reg</t>
+  </si>
+  <si>
+    <t>3A Fuse for 12V</t>
+  </si>
+  <si>
+    <t>3.3V LED Resistor</t>
+  </si>
+  <si>
+    <t>5V LED Resistor</t>
+  </si>
+  <si>
+    <t>12V LED Resistor</t>
+  </si>
+  <si>
+    <t>Indicator LED</t>
+  </si>
+  <si>
+    <t>Fuse, PTC</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>Diode, LED</t>
+  </si>
+  <si>
+    <t>507-1763-1-ND</t>
+  </si>
+  <si>
+    <t>PTC RESET FUSE 16V 750MA 1812</t>
+  </si>
+  <si>
+    <t>750mA Fuse for 3.3 and 5V</t>
+  </si>
+  <si>
+    <t>1A Fuse for 3.3 and 5V, alternate part</t>
+  </si>
+  <si>
+    <t>507-1761-1-ND</t>
+  </si>
+  <si>
+    <t>PTC RESET FUSE 16V 500MA 1812</t>
+  </si>
+  <si>
+    <t>PTC RESET FUSE 16V 2A 1812</t>
+  </si>
+  <si>
+    <t>507-2074-1-ND</t>
+  </si>
+  <si>
+    <t>150Ω</t>
+  </si>
+  <si>
+    <t>390Ω</t>
+  </si>
+  <si>
+    <t>1.2k</t>
+  </si>
+  <si>
+    <t>Imported Unchecked</t>
+  </si>
+  <si>
+    <t>Built-In</t>
+  </si>
+  <si>
+    <t>Filter Cap, HF</t>
+  </si>
+  <si>
+    <t>Filter Cap, LF</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>R1206</t>
+  </si>
+  <si>
+    <t>F1812</t>
+  </si>
+  <si>
+    <t>3mm LED</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>From Motor Driver BOM</t>
+  </si>
+  <si>
+    <t>587-2985-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1007-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +319,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,7 +354,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -217,13 +364,29 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF68282"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -249,10 +412,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -517,11 +676,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBC1D7F-33C6-449F-B668-8911A6B50B6B}">
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +740,772 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f t="shared" ref="I2:I35" si="0">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G2), G2)</f>
+        <v>AP2114HA-3.3TRG1DICT-ND</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="L2" s="3">
+        <f>J2*K2</f>
+        <v>0.36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>102-5018-ND</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2.96</v>
+      </c>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L35" si="1">J3*K3</f>
+        <v>5.92</v>
+      </c>
+      <c r="N3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>507-1761-1-ND</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="N4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>507-1763-1-ND</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="N5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>507-2074-1-ND</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.42</v>
+      </c>
+      <c r="N6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="2">
+        <f>HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G10), G10)</f>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3">
+        <f>J10*K10</f>
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <f t="shared" ref="I11:I12" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G11), G11)</f>
+        <v>1276-1007-1-ND</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" ref="L11:L12" si="3">J11*K11</f>
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>587-2985-1-ND</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E23" s="5"/>
+      <c r="I23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E26" s="5"/>
+      <c r="I26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E27" s="5"/>
+      <c r="I27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E28" s="5"/>
+      <c r="I28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="4"/>
+    </row>
+    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="I32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K36" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="3">
+        <f>SUM($L$2:$L$35)</f>
+        <v>7.54</v>
+      </c>
+    </row>
+    <row r="37" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+    </row>
+    <row r="49" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="L50" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:N36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="N2:N35">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="unchecked">
+      <formula>NOT(ISERROR(SEARCH("unchecked",N2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Need">
+      <formula>NOT(ISERROR(SEARCH("Need",N2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="N2:N35" xr:uid="{A3102630-818A-45FC-B15A-B2D03DE106D7}">
+      <formula1>"Built-In,Imported Unchecked,Built-In Unchecked,Custom,Custom-Unchecked,Needs Model"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N47"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="39.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1071,7 +1996,7 @@
       <c r="L47" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N33"/>
+  <autoFilter ref="A1:N33" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="N2:N32">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unchecked">
       <formula>NOT(ISERROR(SEARCH("unchecked",N2)))</formula>
@@ -1081,12 +2006,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="N2:N32">
+    <dataValidation type="list" allowBlank="1" sqref="N2:N32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Built-In,Imported Unchecked,Built-In Unchecked,Custom,Custom-Unchecked,Needs Model"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Board mostly routed! Added heatsink 3.3V version
</commit_message>
<xml_diff>
--- a/BOM_Initial.xlsx
+++ b/BOM_Initial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Gilliland\Desktop\All Projects\benchBoddy\benchBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABCD03D-FCC5-4FA7-B5B1-20211BB66EC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B7ECC0-9C49-4598-8C3C-A0FBFD1017FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,9 +158,6 @@
     <t>AP2114HA-3.3TRG1DICT-ND</t>
   </si>
   <si>
-    <t>Custom-Unchecked</t>
-  </si>
-  <si>
     <t>102-5018-ND</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>1276-1007-1-ND</t>
+  </si>
+  <si>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,24 +770,24 @@
         <v>0.36</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" si="0"/>
@@ -804,24 +804,24 @@
         <v>5.92</v>
       </c>
       <c r="N3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -838,24 +838,24 @@
         <v>0.42000000000000004</v>
       </c>
       <c r="N4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -872,24 +872,24 @@
         <v>0.42000000000000004</v>
       </c>
       <c r="N5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" t="s">
         <v>60</v>
-      </c>
-      <c r="G6" t="s">
-        <v>61</v>
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -906,21 +906,21 @@
         <v>0.42</v>
       </c>
       <c r="N6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
@@ -935,21 +935,21 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G8" s="8"/>
       <c r="I8" s="2">
@@ -965,21 +965,21 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="0"/>
@@ -994,18 +994,18 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I10" s="2">
         <f>HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G10), G10)</f>
@@ -1020,27 +1020,27 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" ref="I11:I12" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G11), G11)</f>
@@ -1057,27 +1057,27 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>76</v>
-      </c>
-      <c r="G12" t="s">
-        <v>77</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1094,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Filled out MCU Board BOM. Nearly complete BOM except Passives
</commit_message>
<xml_diff>
--- a/BOM_Initial.xlsx
+++ b/BOM_Initial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Gilliland\Desktop\All Projects\benchBoddy\benchBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B7ECC0-9C49-4598-8C3C-A0FBFD1017FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88A3DCA-5EA9-4AEE-A113-AEC5F36DB9F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board Additions" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Board Additions'!$A$1:$N$36</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCU Board'!$A$1:$N$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCU Board'!$A$1:$N$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
   <si>
     <t>Usage</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>3.3V Regulator</t>
-  </si>
-  <si>
     <t>PIC16F1779-I/PT-ND</t>
   </si>
   <si>
@@ -104,27 +101,9 @@
     <t>44-TQFP</t>
   </si>
   <si>
-    <t>576-4766-1-ND</t>
-  </si>
-  <si>
-    <t>IC REG LINEAR 3.3V 500mA</t>
-  </si>
-  <si>
-    <t>6-TDFN</t>
-  </si>
-  <si>
     <t>USB to UART Adapter</t>
   </si>
   <si>
-    <t>AIN protection diodes</t>
-  </si>
-  <si>
-    <t>Voltage Divider Resistors for AINs</t>
-  </si>
-  <si>
-    <t>Passive, Resistor</t>
-  </si>
-  <si>
     <t>Diode</t>
   </si>
   <si>
@@ -273,6 +252,117 @@
   </si>
   <si>
     <t>Custom</t>
+  </si>
+  <si>
+    <t>Microcontroller, Arduino</t>
+  </si>
+  <si>
+    <t>Crystal Oscillator</t>
+  </si>
+  <si>
+    <t>ATMega328P</t>
+  </si>
+  <si>
+    <t>Voltage Reference</t>
+  </si>
+  <si>
+    <t>576-1048-1-ND</t>
+  </si>
+  <si>
+    <t>Op Amp for AINs</t>
+  </si>
+  <si>
+    <t>DAC Chip</t>
+  </si>
+  <si>
+    <t>MCP4728-E/UN-ND</t>
+  </si>
+  <si>
+    <t>LM324DR2GOSCT-ND</t>
+  </si>
+  <si>
+    <t>5V Supply</t>
+  </si>
+  <si>
+    <t>AZ1117IH-5.0TRG1DICT-ND</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 5V 800MA SOT223</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>336-5888-1-ND</t>
+  </si>
+  <si>
+    <t>1727-1582-1-ND</t>
+  </si>
+  <si>
+    <t>5V/AIN/USB protection diodes</t>
+  </si>
+  <si>
+    <t>8MHz</t>
+  </si>
+  <si>
+    <t>887-2015-ND</t>
+  </si>
+  <si>
+    <t>Crystal Capacitors</t>
+  </si>
+  <si>
+    <t>Amp Resistors</t>
+  </si>
+  <si>
+    <t>10k 1%</t>
+  </si>
+  <si>
+    <t>30.1k 1%</t>
+  </si>
+  <si>
+    <t>15k 1%</t>
+  </si>
+  <si>
+    <t>47k 1%</t>
+  </si>
+  <si>
+    <t>Vref Resistor</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>ATMEGA328PB-AURCT-ND</t>
+  </si>
+  <si>
+    <t>Power Filter Caps</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>FTDI Header</t>
+  </si>
+  <si>
+    <t>USB Port</t>
+  </si>
+  <si>
+    <t>Mating Header</t>
+  </si>
+  <si>
+    <t>Reset button</t>
+  </si>
+  <si>
+    <t>Output Header, AIN</t>
+  </si>
+  <si>
+    <t>Output Header, DIO</t>
+  </si>
+  <si>
+    <t>DIO Protection resistors</t>
   </si>
 </sst>
 </file>
@@ -282,7 +372,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +421,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -354,7 +451,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -366,6 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -679,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBC1D7F-33C6-449F-B668-8911A6B50B6B}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,19 +839,19 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I2" s="2" t="str">
         <f t="shared" ref="I2:I35" si="0">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G2), G2)</f>
@@ -770,24 +868,24 @@
         <v>0.36</v>
       </c>
       <c r="N2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" si="0"/>
@@ -804,24 +902,24 @@
         <v>5.92</v>
       </c>
       <c r="N3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
         <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" t="s">
-        <v>57</v>
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -838,24 +936,24 @@
         <v>0.42000000000000004</v>
       </c>
       <c r="N4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -872,24 +970,24 @@
         <v>0.42000000000000004</v>
       </c>
       <c r="N5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -906,21 +1004,21 @@
         <v>0.42</v>
       </c>
       <c r="N6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
@@ -935,21 +1033,21 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G8" s="8"/>
       <c r="I8" s="2">
@@ -965,21 +1063,21 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="0"/>
@@ -994,18 +1092,18 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I10" s="2">
         <f>HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G10), G10)</f>
@@ -1020,27 +1118,27 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
         <v>66</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" t="s">
         <v>68</v>
       </c>
-      <c r="D11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" t="s">
-        <v>75</v>
-      </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" ref="I11:I12" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G11), G11)</f>
@@ -1057,27 +1155,27 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
         <v>68</v>
       </c>
-      <c r="D12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="G12" t="s">
         <v>69</v>
-      </c>
-      <c r="F12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" t="s">
-        <v>76</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1094,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1443,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,491 +1611,703 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="3">
         <v>2.82</v>
       </c>
       <c r="L2" s="3">
         <f>J2*K2</f>
-        <v>2.82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I32" si="0">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
-        <v>576-4766-1-ND</v>
+        <f t="shared" ref="I3:I7" si="0">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
+        <v>AZ1117IH-5.0TRG1DICT-ND</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" s="3">
-        <v>0.2</v>
+        <v>0.36</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L32" si="1">J3*K3</f>
-        <v>0.4</v>
+        <f t="shared" ref="L3:L9" si="1">J3*K3</f>
+        <v>0.36</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ATMEGA328PB-AURCT-ND</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="3">
+        <v>1.42</v>
+      </c>
       <c r="L4" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>887-2015-ND</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.3</v>
+      </c>
       <c r="L5" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="I6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>576-1048-1-ND</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="L6" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>LM324DR2GOSCT-ND</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <f t="shared" ref="I8:I35" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G8), G8)</f>
+        <v>MCP4728-E/UN-ND</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7">
+      <c r="G9" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>336-5888-1-ND</v>
+      </c>
+      <c r="J9">
         <v>1</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K9" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="1"/>
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
         <v>0.69</v>
       </c>
-      <c r="L7" s="3">
-        <f t="shared" si="1"/>
+      <c r="L10" s="3">
+        <f t="shared" ref="L10:L35" si="3">J10*K10</f>
         <v>0.69</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="3"/>
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1727-1582-1-ND</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.31</v>
+      </c>
       <c r="L11" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.92999999999999994</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
       <c r="I12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>92</v>
+      </c>
       <c r="I13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>94</v>
+      </c>
       <c r="I14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>93</v>
+      </c>
       <c r="I15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>95</v>
+      </c>
       <c r="I16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
       <c r="I17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K17" s="3"/>
-      <c r="L17" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
       <c r="I18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>100</v>
+      </c>
       <c r="I19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E20" s="5"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
       <c r="I20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
       <c r="I21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>104</v>
+      </c>
       <c r="I22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="4"/>
-    </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="I23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E24" s="5"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
       <c r="I24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E25" s="5"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>106</v>
+      </c>
       <c r="I25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="5"/>
       <c r="I26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="4"/>
-    </row>
-    <row r="27" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E27" s="5"/>
       <c r="I27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="4"/>
-    </row>
-    <row r="28" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E28" s="5"/>
       <c r="I28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K33" s="6" t="s">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I33" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I34" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I35" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L33" s="3">
-        <f>SUM($L$2:$L$32)</f>
-        <v>3.9099999999999997</v>
-      </c>
-    </row>
-    <row r="34" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-    </row>
-    <row r="35" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-    </row>
-    <row r="37" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="L36" s="3">
+        <f>SUM($L$2:$L$35)</f>
+        <v>6.0399999999999991</v>
+      </c>
+    </row>
+    <row r="37" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
+    <row r="48" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+    </row>
+    <row r="49" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+    </row>
+    <row r="50" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="L50" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N33" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="N2:N32">
+  <autoFilter ref="A1:N36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="N2:N35">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unchecked">
       <formula>NOT(ISERROR(SEARCH("unchecked",N2)))</formula>
     </cfRule>
@@ -2006,7 +2316,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="N2:N32" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="N2:N35" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Built-In,Imported Unchecked,Built-In Unchecked,Custom,Custom-Unchecked,Needs Model"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added components to library and schem
</commit_message>
<xml_diff>
--- a/BOM_Initial.xlsx
+++ b/BOM_Initial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Gilliland\Desktop\All Projects\benchBuddy\benchBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D38988-34DF-4B98-8622-78C15067F238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FE2E6F-1B75-4FC9-AD2D-FEAB72E6C8A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Board Additions'!$A$1:$N$36</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCU Board'!$A$1:$N$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCU Board'!$A$1:$N$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="119">
   <si>
     <t>Usage</t>
   </si>
@@ -113,9 +113,6 @@
     <t>UART Optoisolator</t>
   </si>
   <si>
-    <t>digikey.com/product-detail/en/everlight-electronics-co-ltd/H11L1S-TA/1080-1201-1-ND/2675935</t>
-  </si>
-  <si>
     <t>1080-1201-1-ND</t>
   </si>
   <si>
@@ -332,9 +329,6 @@
     <t>10nF</t>
   </si>
   <si>
-    <t>FTDI Header</t>
-  </si>
-  <si>
     <t>USB Port</t>
   </si>
   <si>
@@ -372,6 +366,33 @@
   </si>
   <si>
     <t>R0805</t>
+  </si>
+  <si>
+    <t>22pF</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>14-SOIC</t>
+  </si>
+  <si>
+    <t>10-MSOP</t>
+  </si>
+  <si>
+    <t>Verify with box</t>
+  </si>
+  <si>
+    <t>6-SMD</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Verify same as USB Motor Driver</t>
+  </si>
+  <si>
+    <t>ICSP Header</t>
   </si>
 </sst>
 </file>
@@ -477,7 +498,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -485,7 +506,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -867,20 +887,20 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>32</v>
       </c>
       <c r="I2" s="2" t="str">
         <f t="shared" ref="I2:I35" si="0">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G2), G2)</f>
@@ -897,24 +917,24 @@
         <v>0.36</v>
       </c>
       <c r="N2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>36</v>
       </c>
+      <c r="B3" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" si="0"/>
@@ -931,24 +951,24 @@
         <v>5.92</v>
       </c>
       <c r="N3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -965,24 +985,24 @@
         <v>0.42000000000000004</v>
       </c>
       <c r="N4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -999,24 +1019,24 @@
         <v>0.42000000000000004</v>
       </c>
       <c r="N5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" t="s">
         <v>105</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" t="s">
-        <v>107</v>
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1033,21 +1053,21 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="N6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
@@ -1062,23 +1082,23 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="8"/>
+        <v>59</v>
+      </c>
+      <c r="G8" s="7"/>
       <c r="I8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1092,21 +1112,21 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="0"/>
@@ -1121,18 +1141,18 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I10" s="2">
         <f>HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G10), G10)</f>
@@ -1147,27 +1167,27 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" ref="I11:I12" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G11), G11)</f>
@@ -1184,27 +1204,27 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>65</v>
-      </c>
-      <c r="G12" t="s">
-        <v>66</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1221,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1570,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,7 +1608,7 @@
     <col min="14" max="14" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1632,51 +1652,51 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="12">
-        <v>0</v>
-      </c>
-      <c r="K2" s="14">
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="13">
         <v>2.82</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="13">
         <f>J2*K2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" ref="I3:I8" si="0">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
@@ -1693,21 +1713,21 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1723,22 +1743,28 @@
         <f t="shared" si="1"/>
         <v>1.42</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1754,12 +1780,24 @@
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" t="s">
         <v>58</v>
       </c>
       <c r="I6" s="2">
@@ -1774,17 +1812,26 @@
         <f>J6*K6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1801,15 +1848,18 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1825,19 +1875,25 @@
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I9" s="2" t="str">
-        <f t="shared" ref="I9:I35" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G9), G9)</f>
+        <f t="shared" ref="I9:I34" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G9), G9)</f>
         <v>MCP4728-E/UN-ND</v>
       </c>
       <c r="J9">
@@ -1850,16 +1906,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>82</v>
+      <c r="G10" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="I10" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1875,23 +1934,30 @@
         <f t="shared" si="1"/>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
+      <c r="D11" t="s">
+        <v>115</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>25</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1080-1201-1-ND</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1900,19 +1966,19 @@
         <v>0.69</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" ref="L11:L35" si="3">J11*K11</f>
+        <f t="shared" ref="L11:L34" si="3">J11*K11</f>
         <v>0.69</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1928,19 +1994,22 @@
         <f t="shared" si="3"/>
         <v>0.92999999999999994</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
         <v>87</v>
       </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>88</v>
-      </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="2"/>
@@ -1952,18 +2021,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="2"/>
@@ -1975,18 +2044,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="2"/>
@@ -1998,18 +2067,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="2"/>
@@ -2021,18 +2090,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17">
         <v>100</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="2"/>
@@ -2041,18 +2110,18 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
         <v>92</v>
       </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>93</v>
-      </c>
       <c r="E18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="2"/>
@@ -2064,18 +2133,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
         <v>95</v>
       </c>
-      <c r="B19" t="s">
+      <c r="E19" t="s">
         <v>58</v>
-      </c>
-      <c r="D19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="2"/>
@@ -2087,18 +2156,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
         <v>58</v>
-      </c>
-      <c r="D20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" t="s">
-        <v>59</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="2"/>
@@ -2110,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -2124,10 +2193,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>100</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E22" s="5"/>
       <c r="I22" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2137,12 +2207,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="5"/>
       <c r="I23" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2153,9 +2225,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="2"/>
@@ -2166,11 +2238,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>102</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E25" s="5"/>
       <c r="I25" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2180,11 +2254,10 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N25" s="4"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E26" s="5"/>
       <c r="I26" s="2">
@@ -2197,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E27" s="5"/>
       <c r="I27" s="2">
         <f t="shared" si="2"/>
@@ -2209,8 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E28" s="5"/>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I28" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2220,8 +2292,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I29" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2233,7 +2306,7 @@
       </c>
       <c r="N29" s="4"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I30" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2243,9 +2316,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N30" s="4"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I31" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2256,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I32" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2290,24 +2362,17 @@
       </c>
     </row>
     <row r="35" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I35" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="3"/>
+      <c r="K35" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="L35" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM($L$2:$L$34)</f>
+        <v>6.0399999999999991</v>
       </c>
     </row>
     <row r="36" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="K36" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L36" s="3">
-        <f>SUM($L$2:$L$35)</f>
-        <v>6.0399999999999991</v>
-      </c>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
     </row>
     <row r="37" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K37" s="3"/>
@@ -2357,16 +2422,12 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K49" s="3"/>
+    <row r="49" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="L50" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:N36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="N2:N35">
+  <autoFilter ref="A1:N35" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="N2:N34">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unchecked">
       <formula>NOT(ISERROR(SEARCH("unchecked",N2)))</formula>
     </cfRule>
@@ -2374,8 +2435,8 @@
       <formula>NOT(ISERROR(SEARCH("Need",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" sqref="N2:N35" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="N2:N34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Built-In,Imported Unchecked,Built-In Unchecked,Custom,Custom-Unchecked,Needs Model"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added analog circuitry. Most of schem is done. Still must do optoisolation and DIO protection
</commit_message>
<xml_diff>
--- a/BOM_Initial.xlsx
+++ b/BOM_Initial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Gilliland\Desktop\All Projects\benchBuddy\benchBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B444105B-F22C-4AA3-B93A-1A772373203A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F788206-3D02-47D9-B0E8-A85B71793D6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Board Additions'!$A$1:$N$36</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCU Board'!$A$1:$N$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCU Board'!$A$1:$N$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="129">
   <si>
     <t>Usage</t>
   </si>
@@ -386,9 +386,6 @@
     <t>6-SMD</t>
   </si>
   <si>
-    <t>In</t>
-  </si>
-  <si>
     <t>Verify same as USB Motor Driver</t>
   </si>
   <si>
@@ -411,6 +408,21 @@
   </si>
   <si>
     <t>Button</t>
+  </si>
+  <si>
+    <t>Op Amp Power Supply</t>
+  </si>
+  <si>
+    <t>SOT89-3</t>
+  </si>
+  <si>
+    <t>497-1192-1-ND</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 9V 100MA SOT89-3</t>
+  </si>
+  <si>
+    <t>L78L09ACUTR</t>
   </si>
 </sst>
 </file>
@@ -1608,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1638,7 @@
     <col min="14" max="14" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1670,7 +1682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
@@ -1700,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1717,7 +1729,7 @@
         <v>78</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I8" si="0">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
+        <f t="shared" ref="I3:I9" si="0">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
         <v>AZ1117IH-5.0TRG1DICT-ND</v>
       </c>
       <c r="J3">
@@ -1727,11 +1739,11 @@
         <v>0.36</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L10" si="1">J3*K3</f>
+        <f t="shared" ref="L3:L11" si="1">J3*K3</f>
         <v>0.36</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1764,11 +1776,8 @@
       <c r="N4" t="s">
         <v>54</v>
       </c>
-      <c r="O4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -1801,11 +1810,8 @@
       <c r="N5" t="s">
         <v>54</v>
       </c>
-      <c r="O5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -1833,11 +1839,8 @@
       <c r="N6" t="s">
         <v>54</v>
       </c>
-      <c r="O6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1847,7 +1850,6 @@
       <c r="D7" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="2"/>
       <c r="G7" t="s">
         <v>72</v>
       </c>
@@ -1869,180 +1871,194 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>125</v>
+      </c>
+      <c r="F8" t="s">
+        <v>127</v>
       </c>
       <c r="G8" t="s">
-        <v>76</v>
+        <v>126</v>
+      </c>
+      <c r="H8" t="s">
+        <v>128</v>
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>LM324DR2GOSCT-ND</v>
+        <v>497-1192-1-ND</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="3">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="L8" s="3">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="N8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>LM324DR2GOSCT-ND</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
         <v>113</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>75</v>
       </c>
-      <c r="I9" s="2" t="str">
-        <f t="shared" ref="I9:I34" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G9), G9)</f>
+      <c r="I10" s="2" t="str">
+        <f t="shared" ref="I10:I35" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G10), G10)</f>
         <v>MCP4728-E/UN-ND</v>
       </c>
-      <c r="J9">
+      <c r="J10">
         <v>1</v>
       </c>
-      <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="2" t="str">
+      <c r="I11" s="2" t="str">
         <f t="shared" si="2"/>
         <v>336-5888-1-ND</v>
       </c>
-      <c r="J10">
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K11" s="3">
         <v>1.35</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L11" s="3">
         <f t="shared" si="1"/>
         <v>1.35</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>115</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="I12" s="2" t="str">
         <f t="shared" si="2"/>
         <v>1080-1201-1-ND</v>
       </c>
-      <c r="J11">
+      <c r="J12">
         <v>1</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K12" s="3">
         <v>0.69</v>
       </c>
-      <c r="L11" s="3">
-        <f t="shared" ref="L11:L34" si="3">J11*K11</f>
+      <c r="L12" s="3">
+        <f t="shared" ref="L12:L35" si="3">J12*K12</f>
         <v>0.69</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>83</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>82</v>
       </c>
-      <c r="I12" s="2" t="str">
+      <c r="I13" s="2" t="str">
         <f t="shared" si="2"/>
         <v>1727-1582-1-ND</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <v>3</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K13" s="3">
         <v>0.31</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L13" s="3">
         <f t="shared" si="3"/>
         <v>0.92999999999999994</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" t="s">
-        <v>109</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -2050,7 +2066,7 @@
         <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
         <v>109</v>
@@ -2065,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -2073,7 +2089,7 @@
         <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
         <v>109</v>
@@ -2088,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -2096,7 +2112,7 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
         <v>109</v>
@@ -2113,13 +2129,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="D17">
-        <v>100</v>
+      <c r="D17" t="s">
+        <v>90</v>
       </c>
       <c r="E17" t="s">
         <v>109</v>
@@ -2129,17 +2145,20 @@
         <v>0</v>
       </c>
       <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="L17" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" t="s">
-        <v>92</v>
+      <c r="D18">
+        <v>100</v>
       </c>
       <c r="E18" t="s">
         <v>109</v>
@@ -2149,23 +2168,20 @@
         <v>0</v>
       </c>
       <c r="K18" s="3"/>
-      <c r="L18" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="2"/>
@@ -2185,7 +2201,7 @@
         <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E20" t="s">
         <v>58</v>
@@ -2202,7 +2218,16 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="2"/>
@@ -2216,9 +2241,8 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>97</v>
-      </c>
-      <c r="E22" s="5"/>
+        <v>98</v>
+      </c>
       <c r="I22" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2228,64 +2252,63 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O22" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="I23" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>99</v>
       </c>
-      <c r="B23" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="B24" t="s">
         <v>123</v>
       </c>
-      <c r="F23" t="s">
+      <c r="E24" t="s">
         <v>122</v>
       </c>
-      <c r="G23" t="s">
+      <c r="F24" t="s">
         <v>121</v>
       </c>
-      <c r="I23" s="2" t="str">
+      <c r="G24" t="s">
+        <v>120</v>
+      </c>
+      <c r="I24" s="2" t="str">
         <f t="shared" si="2"/>
         <v>CKN12220-1-ND</v>
       </c>
-      <c r="J23">
+      <c r="J24">
         <v>1</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K24" s="3">
         <v>0.1</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L24" s="3">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" t="s">
-        <v>120</v>
-      </c>
-      <c r="I24" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N24" s="4"/>
-    </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="F25" t="s">
+        <v>119</v>
+      </c>
       <c r="I25" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2295,15 +2318,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" t="s">
-        <v>119</v>
-      </c>
       <c r="I26" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2315,7 +2336,13 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>117</v>
+      </c>
       <c r="E27" s="5"/>
+      <c r="F27" t="s">
+        <v>118</v>
+      </c>
       <c r="I27" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2327,6 +2354,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E28" s="5"/>
       <c r="I28" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2336,7 +2364,6 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N28" s="4"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I29" s="2">
@@ -2360,6 +2387,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I31" s="2">
@@ -2406,17 +2434,24 @@
       </c>
     </row>
     <row r="35" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="K35" s="6" t="s">
+      <c r="I35" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="K36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L35" s="3">
-        <f>SUM($L$2:$L$34)</f>
-        <v>6.1399999999999988</v>
-      </c>
-    </row>
-    <row r="36" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
+      <c r="L36" s="3">
+        <f>SUM($L$2:$L$35)</f>
+        <v>6.5399999999999991</v>
+      </c>
     </row>
     <row r="37" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K37" s="3"/>
@@ -2466,12 +2501,16 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
+    <row r="50" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="L50" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N35" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="N2:N34">
+  <autoFilter ref="A1:N36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="N2:N35">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unchecked">
       <formula>NOT(ISERROR(SEARCH("unchecked",N2)))</formula>
     </cfRule>
@@ -2480,7 +2519,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="N2:N34" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="N2:N35" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Built-In,Imported Unchecked,Built-In Unchecked,Custom,Custom-Unchecked,Needs Model"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Spec'd header part. Added DIO protection diodes and resistors. Significantly more routing done
</commit_message>
<xml_diff>
--- a/BOM_Initial.xlsx
+++ b/BOM_Initial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Gilliland\Desktop\All Projects\benchBuddy\benchBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F788206-3D02-47D9-B0E8-A85B71793D6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F79A74-014E-43B0-9851-BBE915965ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="2505" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board Additions" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="131">
   <si>
     <t>Usage</t>
   </si>
@@ -423,6 +423,12 @@
   </si>
   <si>
     <t>L78L09ACUTR</t>
+  </si>
+  <si>
+    <t>ED1543-ND</t>
+  </si>
+  <si>
+    <t>5x2 header, 0.1", for analogs</t>
   </si>
 </sst>
 </file>
@@ -1622,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,14 +2331,25 @@
         <v>101</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="I26" s="2">
+      <c r="F26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G26" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="3"/>
+        <v>ED1543-ND</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.28000000000000003</v>
+      </c>
       <c r="L26" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2450,7 +2467,7 @@
       </c>
       <c r="L36" s="3">
         <f>SUM($L$2:$L$35)</f>
-        <v>6.5399999999999991</v>
+        <v>6.8199999999999994</v>
       </c>
     </row>
     <row r="37" spans="9:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Exported BOM from eagle. Spec'd resistors
</commit_message>
<xml_diff>
--- a/BOM_Initial.xlsx
+++ b/BOM_Initial.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Gilliland\Desktop\All Projects\benchBuddy\benchBuddy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\EENG393\Projects\benchBuddy\benchBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F79A74-014E-43B0-9851-BBE915965ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="2505" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="2505" windowWidth="21600" windowHeight="11385" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main Board Additions" sheetId="3" r:id="rId1"/>
     <sheet name="MCU Board" sheetId="2" r:id="rId2"/>
+    <sheet name="benchBuddyPSB_BOM" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Main Board Additions'!$A$1:$N$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MCU Board'!$A$1:$N$36</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="257">
   <si>
     <t>Usage</t>
   </si>
@@ -429,12 +430,390 @@
   </si>
   <si>
     <t>5x2 header, 0.1", for analogs</t>
+  </si>
+  <si>
+    <t>Have</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Parts</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>CPOL-USB</t>
+  </si>
+  <si>
+    <t>PANASONIC_B</t>
+  </si>
+  <si>
+    <t>C1, C2, C3</t>
+  </si>
+  <si>
+    <t>POLARIZED CAPACITOR, American symbol</t>
+  </si>
+  <si>
+    <t>10n</t>
+  </si>
+  <si>
+    <t>C-USC1206</t>
+  </si>
+  <si>
+    <t>C1206</t>
+  </si>
+  <si>
+    <t>C4, C6</t>
+  </si>
+  <si>
+    <t>CAPACITOR, American symbol</t>
+  </si>
+  <si>
+    <t>2.2u</t>
+  </si>
+  <si>
+    <t>C5, C7</t>
+  </si>
+  <si>
+    <t>C-USC0805</t>
+  </si>
+  <si>
+    <t>C8, C11, C13</t>
+  </si>
+  <si>
+    <t>C9, C10, C12, C14</t>
+  </si>
+  <si>
+    <t>LED3MM</t>
+  </si>
+  <si>
+    <t>LED_3MM</t>
+  </si>
+  <si>
+    <t>D1, D2, D3</t>
+  </si>
+  <si>
+    <t>LED (Generic)</t>
+  </si>
+  <si>
+    <t>4A It</t>
+  </si>
+  <si>
+    <t>FUSE</t>
+  </si>
+  <si>
+    <t>LITTELFUSE_MINISMDC260F/12-2</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>1.5A It</t>
+  </si>
+  <si>
+    <t>F2, F3</t>
+  </si>
+  <si>
+    <t>TLC274D</t>
+  </si>
+  <si>
+    <t>SO14</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>OP AMP</t>
+  </si>
+  <si>
+    <t>LM334Z</t>
+  </si>
+  <si>
+    <t>TO92</t>
+  </si>
+  <si>
+    <t>IC3</t>
+  </si>
+  <si>
+    <t>3-Terminal Adjustable Current Sources</t>
+  </si>
+  <si>
+    <t>LM324D</t>
+  </si>
+  <si>
+    <t>IC4, IC5</t>
+  </si>
+  <si>
+    <t>12V_DC</t>
+  </si>
+  <si>
+    <t>POWER_JACKSLT</t>
+  </si>
+  <si>
+    <t>POWER_JACK_SLOT</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Power Jack Connector</t>
+  </si>
+  <si>
+    <t>PHOENIX_SPRING_TERM_2POS</t>
+  </si>
+  <si>
+    <t>SPRING_TERM_2POS</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>PINHD-1X6</t>
+  </si>
+  <si>
+    <t>1X06</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>PIN HEADER</t>
+  </si>
+  <si>
+    <t>JP1E</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>JP1, JP2</t>
+  </si>
+  <si>
+    <t>JUMPER</t>
+  </si>
+  <si>
+    <t>SK104-PAD</t>
+  </si>
+  <si>
+    <t>KK1</t>
+  </si>
+  <si>
+    <t>HEATSINK manufacturer Fischer/distributor Buerklin</t>
+  </si>
+  <si>
+    <t>LEDCHIPLED_1206</t>
+  </si>
+  <si>
+    <t>CHIPLED_1206</t>
+  </si>
+  <si>
+    <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8, LED9</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>P78E05-1000</t>
+  </si>
+  <si>
+    <t>CONV_P78E05-1000</t>
+  </si>
+  <si>
+    <t>PS1, PS2</t>
+  </si>
+  <si>
+    <t>NON-ISOLATED DC SWITCHING REGULATOR</t>
+  </si>
+  <si>
+    <t>600mA/40V</t>
+  </si>
+  <si>
+    <t>TRANS_NPN-MMBT2222AL</t>
+  </si>
+  <si>
+    <t>SOT23-3</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>NPN transistor</t>
+  </si>
+  <si>
+    <t>2.2kÎ©</t>
+  </si>
+  <si>
+    <t>R-US_R1206</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>RESISTOR, American symbol</t>
+  </si>
+  <si>
+    <t>10kÎ©</t>
+  </si>
+  <si>
+    <t>R17, R18, R20, R21</t>
+  </si>
+  <si>
+    <t>1Î©</t>
+  </si>
+  <si>
+    <t>R-US_0411/15</t>
+  </si>
+  <si>
+    <t>0411/15</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>EVUF2A</t>
+  </si>
+  <si>
+    <t>EVUF</t>
+  </si>
+  <si>
+    <t>R2, R22</t>
+  </si>
+  <si>
+    <t>9 mm Square Rotary Potentiometers</t>
+  </si>
+  <si>
+    <t>68Î©</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R31, R32, R33</t>
+  </si>
+  <si>
+    <t>1kÎ©</t>
+  </si>
+  <si>
+    <t>R4, R5, R16, R23, R24, R25, R26, R27, R28, R29, R30</t>
+  </si>
+  <si>
+    <t>R6, R7, R8, R9, R10, R11, R12, R13, R14, R15</t>
+  </si>
+  <si>
+    <t>SWITCH-DPDT-SMD-AYZ0202</t>
+  </si>
+  <si>
+    <t>SWITCH_DPDT_SMD_AYZ0202</t>
+  </si>
+  <si>
+    <t>S1, S2, S3</t>
+  </si>
+  <si>
+    <t>Double-Pole, Double-Throw (DPDT) Switch</t>
+  </si>
+  <si>
+    <t>EG2362</t>
+  </si>
+  <si>
+    <t>SWITCH_EG2362-ND</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>LT3080</t>
+  </si>
+  <si>
+    <t>TO-220-5R</t>
+  </si>
+  <si>
+    <t>U$1</t>
+  </si>
+  <si>
+    <t>HEATSINK_MINI</t>
+  </si>
+  <si>
+    <t>U$2, U$3</t>
+  </si>
+  <si>
+    <t>LP2983AIM5-1.0/NOPBMF05A-L</t>
+  </si>
+  <si>
+    <t>MF05A-L</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>LP2985-10DBVR</t>
+  </si>
+  <si>
+    <t>DBV5</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>3V3REG-HEATSINK</t>
+  </si>
+  <si>
+    <t>SOT223-HS</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Cheap 3.3V VReg, Linear SOT223, 1A</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Extra (Re-use)</t>
+  </si>
+  <si>
+    <t>Extra (Bins)</t>
+  </si>
+  <si>
+    <t>Any color LED</t>
+  </si>
+  <si>
+    <t>Extra (Buy)</t>
+  </si>
+  <si>
+    <t>Class and Extra</t>
+  </si>
+  <si>
+    <t>Banana Connectors</t>
+  </si>
+  <si>
+    <t>Selection Switch</t>
+  </si>
+  <si>
+    <t>RMCF1206JT150RCT-ND</t>
+  </si>
+  <si>
+    <t>RES 150 OHM 5% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RMCF1206JT390RCT-ND</t>
+  </si>
+  <si>
+    <t>RES 390 OHM 5% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RMCF1206JT1K20CT-ND</t>
+  </si>
+  <si>
+    <t>RES 1.2K OHM 5% 1/4W 1206</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -534,7 +913,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -549,13 +928,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -859,11 +1246,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBC1D7F-33C6-449F-B668-8911A6B50B6B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,8 +1328,8 @@
       <c r="G2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I35" si="0">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G2), G2)</f>
+      <c r="I2" s="14" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G2), G2)</f>
         <v>AP2114HA-3.3TRG1DICT-ND</v>
       </c>
       <c r="J2">
@@ -972,8 +1362,8 @@
       <c r="G3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="I3" s="14" t="str">
+        <f t="shared" ref="I3:I35" si="0">HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
         <v>102-5018-ND</v>
       </c>
       <c r="J3">
@@ -1006,7 +1396,7 @@
       <c r="G4" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="2" t="str">
+      <c r="I4" s="14" t="str">
         <f t="shared" si="0"/>
         <v>507-1761-1-ND</v>
       </c>
@@ -1040,7 +1430,7 @@
       <c r="G5" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="2" t="str">
+      <c r="I5" s="14" t="str">
         <f t="shared" si="0"/>
         <v>507-1763-1-ND</v>
       </c>
@@ -1074,7 +1464,7 @@
       <c r="G6" t="s">
         <v>105</v>
       </c>
-      <c r="I6" s="2" t="str">
+      <c r="I6" s="14" t="str">
         <f t="shared" si="0"/>
         <v>507-1780-1-ND</v>
       </c>
@@ -1105,17 +1495,25 @@
       <c r="E7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F7" t="s">
+        <v>252</v>
+      </c>
+      <c r="G7" t="s">
+        <v>251</v>
+      </c>
+      <c r="I7" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>RMCF1206JT150RCT-ND</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
       <c r="L7" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="N7" t="s">
         <v>54</v>
@@ -1134,18 +1532,25 @@
       <c r="E8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="I8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F8" t="s">
+        <v>254</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="I8" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>RMCF1206JT390RCT-ND</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
       <c r="L8" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="N8" t="s">
         <v>54</v>
@@ -1164,17 +1569,25 @@
       <c r="E9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F9" t="s">
+        <v>256</v>
+      </c>
+      <c r="G9" t="s">
+        <v>255</v>
+      </c>
+      <c r="I9" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>RMCF1206JT1K20CT-ND</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3">
+        <v>2.8000000000000001E-2</v>
+      </c>
       <c r="L9" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="N9" t="s">
         <v>54</v>
@@ -1190,17 +1603,25 @@
       <c r="E10" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="2">
-        <f>HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G10), G10)</f>
+      <c r="F10" t="s">
+        <v>246</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J10">
         <v>3</v>
       </c>
-      <c r="K10" s="3"/>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
       <c r="L10" s="3">
         <f>J10*K10</f>
         <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>131</v>
       </c>
       <c r="N10" t="s">
         <v>54</v>
@@ -1225,19 +1646,22 @@
       <c r="G11" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="2" t="str">
-        <f t="shared" ref="I11:I12" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G11), G11)</f>
+      <c r="I11" s="14" t="str">
+        <f t="shared" si="0"/>
         <v>1276-1007-1-ND</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11" s="3">
         <v>0</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" ref="L11:L12" si="3">J11*K11</f>
-        <v>0</v>
+        <f t="shared" ref="L11:L12" si="2">J11*K11</f>
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>131</v>
       </c>
       <c r="N11" t="s">
         <v>54</v>
@@ -1262,26 +1686,32 @@
       <c r="G12" t="s">
         <v>65</v>
       </c>
-      <c r="I12" s="2" t="str">
+      <c r="I12" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>587-2985-1-ND</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
         <f t="shared" si="2"/>
-        <v>587-2985-1-ND</v>
-      </c>
-      <c r="J12">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3">
-        <v>0</v>
-      </c>
-      <c r="L12" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
+        <v>131</v>
       </c>
       <c r="N12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I13" s="2">
+      <c r="A13" t="s">
+        <v>250</v>
+      </c>
+      <c r="I13" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1292,7 +1722,10 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I14" s="2">
+      <c r="A14" t="s">
+        <v>249</v>
+      </c>
+      <c r="I14" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1303,7 +1736,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I15" s="2">
+      <c r="I15" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1314,7 +1747,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I16" s="2">
+      <c r="I16" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1325,7 +1758,7 @@
       </c>
     </row>
     <row r="17" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I17" s="2">
+      <c r="I17" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1336,7 +1769,7 @@
       </c>
     </row>
     <row r="18" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I18" s="2">
+      <c r="I18" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1347,7 +1780,7 @@
       </c>
     </row>
     <row r="19" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I19" s="2">
+      <c r="I19" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1358,7 +1791,7 @@
       </c>
     </row>
     <row r="20" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I20" s="2">
+      <c r="I20" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1369,7 +1802,7 @@
       </c>
     </row>
     <row r="21" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I21" s="2">
+      <c r="I21" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1380,7 +1813,7 @@
       </c>
     </row>
     <row r="22" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I22" s="2">
+      <c r="I22" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1392,7 +1825,7 @@
     </row>
     <row r="23" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E23" s="5"/>
-      <c r="I23" s="2">
+      <c r="I23" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1403,7 +1836,7 @@
       </c>
     </row>
     <row r="24" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I24" s="2">
+      <c r="I24" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1414,7 +1847,7 @@
       </c>
     </row>
     <row r="25" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I25" s="2">
+      <c r="I25" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1427,7 +1860,7 @@
     </row>
     <row r="26" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E26" s="5"/>
-      <c r="I26" s="2">
+      <c r="I26" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1439,7 +1872,7 @@
     </row>
     <row r="27" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E27" s="5"/>
-      <c r="I27" s="2">
+      <c r="I27" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1451,7 +1884,7 @@
     </row>
     <row r="28" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E28" s="5"/>
-      <c r="I28" s="2">
+      <c r="I28" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1462,7 +1895,7 @@
       </c>
     </row>
     <row r="29" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I29" s="2">
+      <c r="I29" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1474,7 +1907,7 @@
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I30" s="2">
+      <c r="I30" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1486,7 +1919,7 @@
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I31" s="2">
+      <c r="I31" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1497,7 +1930,7 @@
       </c>
     </row>
     <row r="32" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="I32" s="2">
+      <c r="I32" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1508,7 +1941,7 @@
       </c>
     </row>
     <row r="33" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I33" s="2">
+      <c r="I33" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1519,7 +1952,7 @@
       </c>
     </row>
     <row r="34" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I34" s="2">
+      <c r="I34" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1530,7 +1963,7 @@
       </c>
     </row>
     <row r="35" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I35" s="2">
+      <c r="I35" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1546,7 +1979,7 @@
       </c>
       <c r="L36" s="3">
         <f>SUM($L$2:$L$35)</f>
-        <v>7.68</v>
+        <v>7.7639999999999985</v>
       </c>
     </row>
     <row r="37" spans="9:12" x14ac:dyDescent="0.25">
@@ -1605,17 +2038,17 @@
       <c r="L50" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:N36"/>
   <conditionalFormatting sqref="N2:N35">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="unchecked">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="unchecked">
       <formula>NOT(ISERROR(SEARCH("unchecked",N2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Need">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Need">
       <formula>NOT(ISERROR(SEARCH("Need",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="N2:N35" xr:uid="{A3102630-818A-45FC-B15A-B2D03DE106D7}">
+    <dataValidation type="list" allowBlank="1" sqref="N2:N35">
       <formula1>"Built-In,Imported Unchecked,Built-In Unchecked,Custom,Custom-Unchecked,Needs Model"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1625,11 +2058,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,7 +2171,7 @@
         <v>78</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I9" si="0">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
         <v>AZ1117IH-5.0TRG1DICT-ND</v>
       </c>
       <c r="J3">
@@ -1745,7 +2181,7 @@
         <v>0.36</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" ref="L3:L11" si="1">J3*K3</f>
+        <f t="shared" ref="L3:L11" si="0">J3*K3</f>
         <v>0.36</v>
       </c>
     </row>
@@ -1766,7 +2202,7 @@
         <v>70</v>
       </c>
       <c r="I4" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I4:I35" si="1">HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G4), G4)</f>
         <v>ATMEGA328PB-AURCT-ND</v>
       </c>
       <c r="J4">
@@ -1776,7 +2212,7 @@
         <v>1.42</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.42</v>
       </c>
       <c r="N4" t="s">
@@ -1800,7 +2236,7 @@
         <v>84</v>
       </c>
       <c r="I5" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>887-2015-ND</v>
       </c>
       <c r="J5">
@@ -1810,7 +2246,7 @@
         <v>0.3</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
       <c r="N5" t="s">
@@ -1831,7 +2267,7 @@
         <v>58</v>
       </c>
       <c r="I6" s="2">
-        <f>HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G6), G6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J6">
@@ -1860,7 +2296,7 @@
         <v>72</v>
       </c>
       <c r="I7" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>576-1048-1-ND</v>
       </c>
       <c r="J7">
@@ -1870,7 +2306,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="N7" t="s">
@@ -1897,7 +2333,7 @@
         <v>128</v>
       </c>
       <c r="I8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>497-1192-1-ND</v>
       </c>
       <c r="J8">
@@ -1907,7 +2343,7 @@
         <v>0.4</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="N8" t="s">
@@ -1928,7 +2364,7 @@
         <v>76</v>
       </c>
       <c r="I9" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>LM324DR2GOSCT-ND</v>
       </c>
       <c r="J9">
@@ -1938,7 +2374,7 @@
         <v>0.35</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
       <c r="N9" t="s">
@@ -1959,7 +2395,7 @@
         <v>75</v>
       </c>
       <c r="I10" s="2" t="str">
-        <f t="shared" ref="I10:I35" si="2">HYPERLINK(_xlfn.CONCAT("https://www.digikey.com/products/en?keywords=",G10), G10)</f>
+        <f t="shared" si="1"/>
         <v>MCP4728-E/UN-ND</v>
       </c>
       <c r="J10">
@@ -1969,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M10" t="s">
@@ -1987,7 +2423,7 @@
         <v>81</v>
       </c>
       <c r="I11" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>336-5888-1-ND</v>
       </c>
       <c r="J11">
@@ -1997,7 +2433,7 @@
         <v>1.35</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.35</v>
       </c>
       <c r="N11" t="s">
@@ -2022,7 +2458,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1080-1201-1-ND</v>
       </c>
       <c r="J12">
@@ -2032,7 +2468,7 @@
         <v>0.69</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" ref="L12:L35" si="3">J12*K12</f>
+        <f t="shared" ref="L12:L35" si="2">J12*K12</f>
         <v>0.69</v>
       </c>
     </row>
@@ -2047,7 +2483,7 @@
         <v>82</v>
       </c>
       <c r="I13" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1727-1582-1-ND</v>
       </c>
       <c r="J13">
@@ -2057,7 +2493,7 @@
         <v>0.31</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.92999999999999994</v>
       </c>
       <c r="N13" t="s">
@@ -2078,12 +2514,12 @@
         <v>109</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2101,12 +2537,12 @@
         <v>109</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2124,12 +2560,12 @@
         <v>109</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2147,12 +2583,12 @@
         <v>109</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2170,7 +2606,7 @@
         <v>109</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K18" s="3"/>
@@ -2190,12 +2626,12 @@
         <v>109</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2213,12 +2649,12 @@
         <v>58</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2236,12 +2672,12 @@
         <v>58</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2250,12 +2686,12 @@
         <v>98</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2265,12 +2701,12 @@
       </c>
       <c r="E23" s="5"/>
       <c r="I23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O23" t="s">
@@ -2294,7 +2730,7 @@
         <v>120</v>
       </c>
       <c r="I24" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>CKN12220-1-ND</v>
       </c>
       <c r="J24">
@@ -2304,7 +2740,7 @@
         <v>0.1</v>
       </c>
       <c r="L24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
     </row>
@@ -2316,12 +2752,15 @@
         <v>119</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N25" s="4"/>
@@ -2338,7 +2777,7 @@
         <v>129</v>
       </c>
       <c r="I26" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>ED1543-ND</v>
       </c>
       <c r="J26">
@@ -2348,7 +2787,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="L26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.28000000000000003</v>
       </c>
     </row>
@@ -2361,103 +2800,108 @@
         <v>118</v>
       </c>
       <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E28" s="5"/>
       <c r="I28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N30" s="4"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K34" s="3"/>
       <c r="L34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2526,24 +2970,816 @@
       <c r="L50" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:N36"/>
   <conditionalFormatting sqref="N2:N35">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="unchecked">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="unchecked">
       <formula>NOT(ISERROR(SEARCH("unchecked",N2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Need">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Need">
       <formula>NOT(ISERROR(SEARCH("Need",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="N2:N35" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="N2:N35">
       <formula1>"Built-In,Imported Unchecked,Built-In Unchecked,Custom,Custom-Unchecked,Needs Model"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="59.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" t="s">
+        <v>182</v>
+      </c>
+      <c r="F10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" t="s">
+        <v>186</v>
+      </c>
+      <c r="G11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E12" t="s">
+        <v>189</v>
+      </c>
+      <c r="F12" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E13" t="s">
+        <v>198</v>
+      </c>
+      <c r="F13" t="s">
+        <v>199</v>
+      </c>
+      <c r="G13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
+        <v>203</v>
+      </c>
+      <c r="G14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
+        <v>206</v>
+      </c>
+      <c r="G15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>243</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" t="s">
+        <v>208</v>
+      </c>
+      <c r="E16" t="s">
+        <v>209</v>
+      </c>
+      <c r="F16" t="s">
+        <v>210</v>
+      </c>
+      <c r="G16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E17" t="s">
+        <v>212</v>
+      </c>
+      <c r="F17" t="s">
+        <v>213</v>
+      </c>
+      <c r="G17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>243</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>215</v>
+      </c>
+      <c r="D18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>216</v>
+      </c>
+      <c r="G18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>243</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>217</v>
+      </c>
+      <c r="G19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>218</v>
+      </c>
+      <c r="D20" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
+        <v>219</v>
+      </c>
+      <c r="G20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>243</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" t="s">
+        <v>220</v>
+      </c>
+      <c r="G21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E22" t="s">
+        <v>229</v>
+      </c>
+      <c r="F22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>233</v>
+      </c>
+      <c r="D23" t="s">
+        <v>233</v>
+      </c>
+      <c r="E23" t="s">
+        <v>234</v>
+      </c>
+      <c r="F23" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>236</v>
+      </c>
+      <c r="D24" t="s">
+        <v>236</v>
+      </c>
+      <c r="E24" t="s">
+        <v>237</v>
+      </c>
+      <c r="F24" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>248</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>221</v>
+      </c>
+      <c r="E25" t="s">
+        <v>222</v>
+      </c>
+      <c r="F25" t="s">
+        <v>223</v>
+      </c>
+      <c r="G25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" t="s">
+        <v>151</v>
+      </c>
+      <c r="G26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>245</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>177</v>
+      </c>
+      <c r="E27" t="s">
+        <v>178</v>
+      </c>
+      <c r="F27" t="s">
+        <v>179</v>
+      </c>
+      <c r="G27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E28" t="s">
+        <v>226</v>
+      </c>
+      <c r="F28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>245</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>231</v>
+      </c>
+      <c r="D29" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29" t="s">
+        <v>231</v>
+      </c>
+      <c r="F29" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>247</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>247</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>247</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>192</v>
+      </c>
+      <c r="D32" t="s">
+        <v>192</v>
+      </c>
+      <c r="E32" t="s">
+        <v>193</v>
+      </c>
+      <c r="F32" t="s">
+        <v>194</v>
+      </c>
+      <c r="G32" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>247</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>239</v>
+      </c>
+      <c r="D33" t="s">
+        <v>239</v>
+      </c>
+      <c r="E33" t="s">
+        <v>240</v>
+      </c>
+      <c r="F33" t="s">
+        <v>241</v>
+      </c>
+      <c r="G33" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>244</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" t="s">
+        <v>147</v>
+      </c>
+      <c r="G34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>244</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" t="s">
+        <v>148</v>
+      </c>
+      <c r="G35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:G35">
+    <sortCondition ref="A2:A35"/>
+    <sortCondition ref="F2:F35"/>
+  </sortState>
+  <conditionalFormatting sqref="A2:A35">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="extra">
+      <formula>NOT(ISERROR(SEARCH("extra",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Determined final qtys for ordering
</commit_message>
<xml_diff>
--- a/BOM_Initial.xlsx
+++ b/BOM_Initial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Gilliland\Desktop\All Projects\benchBuddy\benchBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07C6CDA-8465-46E5-82AA-14A42B0C9583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81498D47-0930-42C0-8219-FD00EBEA5D47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PurchaseBOM" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Main Board Additions'!$B$1:$O$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'MCU Board'!$A$1:$N$35</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PurchaseBOM!$B$1:$O$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PurchaseBOM!$A$1:$M$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="356">
   <si>
     <t>Usage</t>
   </si>
@@ -1084,6 +1084,30 @@
   </si>
   <si>
     <t>2057-PH2-06-UA-ND</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Part List</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>PSB</t>
+  </si>
+  <si>
+    <t>MBP</t>
+  </si>
+  <si>
+    <t>Order Qty</t>
+  </si>
+  <si>
+    <t>Qty Required</t>
+  </si>
+  <si>
+    <t>CP2102N-A02-GQFN24R</t>
   </si>
 </sst>
 </file>
@@ -1192,25 +1216,18 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF68282"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1520,56 +1537,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="1" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="39.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>354</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>353</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>10</v>
@@ -1578,1363 +1594,1705 @@
         <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>348</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>226</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="11" t="str">
-        <f t="shared" ref="J2:J13" si="0">HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H2), H2)</f>
-        <v>AP2114HA-3.3TRG1DICT-ND</v>
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G2), G2)</f>
+        <v>CKN12220-1-ND</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
       </c>
       <c r="K2">
+        <f>J2</f>
         <v>1</v>
       </c>
       <c r="L2" s="3">
-        <v>0.36</v>
+        <v>0.1</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" ref="M2:M9" si="1">K2*L2</f>
-        <v>0.36</v>
-      </c>
-      <c r="O2" t="s">
-        <v>60</v>
+        <f>J2*L2</f>
+        <v>0.1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>352</v>
+      </c>
+      <c r="O2" t="str">
+        <f>_xlfn.CONCAT(N2, "-",C2)</f>
+        <v>MBP-S1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>28</v>
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
+        <v>55</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>102-5018-ND</v>
+        <v>59</v>
+      </c>
+      <c r="I3" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
+        <v>1276-1007-1-ND</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
       </c>
       <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="M3" s="3">
+        <f>J3*L3</f>
+        <v>0.12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>352</v>
+      </c>
+      <c r="O3" t="str">
+        <f>_xlfn.CONCAT(N3, "-",C3)</f>
+        <v>MBP-C8, C11, C13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>334</v>
+      </c>
+      <c r="G4" t="s">
+        <v>333</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G4), G4)</f>
+        <v>732-7816-1-ND</v>
+      </c>
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="L3" s="3">
-        <v>2.96</v>
-      </c>
-      <c r="M3" s="3">
-        <f t="shared" si="1"/>
-        <v>5.92</v>
-      </c>
-      <c r="O3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>507-1761-1-ND</v>
-      </c>
       <c r="K4">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L4" s="3">
-        <v>0.14000000000000001</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" si="1"/>
-        <v>0.42000000000000004</v>
-      </c>
-      <c r="O4" t="s">
-        <v>46</v>
+        <f>J4*L4</f>
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>352</v>
+      </c>
+      <c r="O4" t="str">
+        <f>_xlfn.CONCAT(N4, "-",C4)</f>
+        <v>MBP-C1, C2</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>272</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
+        <v>87</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>507-1763-1-ND</v>
+        <v>335</v>
+      </c>
+      <c r="I5" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G5), G5)</f>
+        <v>1276-6471-1-ND</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L5" s="3">
-        <v>0.14000000000000001</v>
+        <v>4.7E-2</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="1"/>
-        <v>0.42000000000000004</v>
-      </c>
-      <c r="O5" t="s">
-        <v>46</v>
+        <f>J5*L5</f>
+        <v>0.188</v>
+      </c>
+      <c r="N5" t="s">
+        <v>352</v>
+      </c>
+      <c r="O5" t="str">
+        <f>_xlfn.CONCAT(N5, "-",C5)</f>
+        <v>MBP-C3, C5, C7, C9</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>312</v>
+      </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>263</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>262</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>338</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" t="s">
-        <v>96</v>
-      </c>
-      <c r="J6" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>507-1780-1-ND</v>
+        <v>337</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G6), G6)</f>
+        <v>732-12256-1-ND</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
       </c>
       <c r="K6">
         <v>2</v>
       </c>
       <c r="L6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M6" s="3">
+        <f>J6*L6</f>
+        <v>0.2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>351</v>
+      </c>
+      <c r="O6" t="str">
+        <f>_xlfn.CONCAT(N6, "-",C6)</f>
+        <v>PSB-C10, C11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>336</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G7), G7)</f>
+        <v>1276-6455-1-ND</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.108</v>
+      </c>
+      <c r="M7" s="3">
+        <f>J7*L7</f>
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="N7" t="s">
+        <v>351</v>
+      </c>
+      <c r="O7" t="str">
+        <f>_xlfn.CONCAT(N7, "-",C7)</f>
+        <v>PSB-C4, C6, C8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>336</v>
+      </c>
+      <c r="I8" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G8), G8)</f>
+        <v>1276-6455-1-ND</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.108</v>
+      </c>
+      <c r="M8" s="3">
+        <f>J8*L8</f>
+        <v>0.432</v>
+      </c>
+      <c r="N8" t="s">
+        <v>352</v>
+      </c>
+      <c r="O8" t="str">
+        <f>_xlfn.CONCAT(N8, "-",C8)</f>
+        <v>MBP-C9, C10, C12, C14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G9), G9)</f>
+        <v>887-2015-ND</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f>J9</f>
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="M9" s="3">
+        <f>J9*L9</f>
+        <v>0.3</v>
+      </c>
+      <c r="N9" t="s">
+        <v>351</v>
+      </c>
+      <c r="O9" t="str">
+        <f>_xlfn.CONCAT(N9, "-",C9)</f>
+        <v>PSB-Q1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G10), G10)</f>
+        <v>102-5018-ND</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <f>J10</f>
+        <v>2</v>
+      </c>
+      <c r="L10" s="3">
+        <v>2.96</v>
+      </c>
+      <c r="M10" s="3">
+        <f>J10*L10</f>
+        <v>5.92</v>
+      </c>
+      <c r="N10" t="s">
+        <v>351</v>
+      </c>
+      <c r="O10" t="str">
+        <f>_xlfn.CONCAT(N10, "-",C10)</f>
+        <v>PSB-PS1, PS2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>296</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G11), G11)</f>
+        <v>576-1048-1-ND</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f>J11</f>
+        <v>1</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M11" s="3">
+        <f>J11*L11</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N11" t="s">
+        <v>351</v>
+      </c>
+      <c r="O11" t="str">
+        <f>_xlfn.CONCAT(N11, "-",C11)</f>
+        <v>PSB-D1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>308</v>
+      </c>
+      <c r="G12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G12), G12)</f>
+        <v>1727-1582-1-ND</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="M12" s="3">
+        <f>J12*L12</f>
+        <v>1.24</v>
+      </c>
+      <c r="N12" t="s">
+        <v>352</v>
+      </c>
+      <c r="O12" t="str">
+        <f>_xlfn.CONCAT(N12, "-",C12)</f>
+        <v>MBP-U4, U7, U8, U9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G13), G13)</f>
+        <v>507-1761-1-ND</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M13" s="3">
+        <f>J13*L13</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="M6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="O6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>246</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" t="s">
-        <v>236</v>
-      </c>
-      <c r="H7" t="s">
-        <v>235</v>
-      </c>
-      <c r="J7" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>RMCF1206JT150RCT-ND</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7" s="3">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="M7" s="3">
-        <f t="shared" si="1"/>
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="O7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s">
-        <v>245</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" t="s">
-        <v>238</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="J8" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>RMCF1206JT390RCT-ND</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8" s="3">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="M8" s="3">
-        <f t="shared" si="1"/>
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="O8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>244</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" t="s">
-        <v>240</v>
-      </c>
-      <c r="H9" t="s">
-        <v>239</v>
-      </c>
-      <c r="J9" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>RMCF1206JT1K20CT-ND</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9" s="3">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="M9" s="3">
-        <f t="shared" si="1"/>
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="O9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>1276-1007-1-ND</v>
-      </c>
-      <c r="K10">
+      <c r="N13" t="s">
+        <v>352</v>
+      </c>
+      <c r="O13" t="str">
+        <f>_xlfn.CONCAT(N13, "-",C13)</f>
+        <v>MBP-F2, F3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G14), G14)</f>
+        <v>507-1763-1-ND</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
         <v>3</v>
       </c>
-      <c r="L10" s="3">
-        <v>0</v>
-      </c>
-      <c r="M10" s="3">
-        <f t="shared" ref="M10:M11" si="2">K10*L10</f>
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
-        <v>116</v>
-      </c>
-      <c r="O10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>133</v>
-      </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>587-2985-1-ND</v>
-      </c>
-      <c r="K11">
-        <v>4</v>
-      </c>
-      <c r="L11" s="3">
-        <v>0</v>
-      </c>
-      <c r="M11" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>234</v>
-      </c>
-      <c r="C12" t="s">
-        <v>319</v>
-      </c>
-      <c r="D12" t="s">
-        <v>241</v>
-      </c>
-      <c r="G12" t="s">
-        <v>318</v>
-      </c>
-      <c r="H12" t="s">
-        <v>317</v>
-      </c>
-      <c r="J12" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>401-2001-ND</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12" s="3">
-        <v>0.43</v>
-      </c>
-      <c r="M12" s="3">
-        <f>K12*L12</f>
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>249</v>
-      </c>
-      <c r="C13" t="s">
-        <v>320</v>
-      </c>
-      <c r="D13" t="s">
-        <v>164</v>
-      </c>
-      <c r="F13" t="s">
-        <v>243</v>
-      </c>
-      <c r="H13" t="s">
-        <v>248</v>
-      </c>
-      <c r="J13" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>2057-PH1-06-UA-ND</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="M13" s="3">
-        <f>K13*L13</f>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>273</v>
-      </c>
-      <c r="E14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" t="s">
-        <v>334</v>
-      </c>
-      <c r="H14" t="s">
-        <v>333</v>
-      </c>
-      <c r="J14" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H14), H14)</f>
-        <v>732-7816-1-ND</v>
-      </c>
-      <c r="K14">
-        <v>2</v>
-      </c>
       <c r="L14" s="3">
-        <v>4.2999999999999997E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M14" s="3">
-        <f>K14*L14</f>
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="O14" t="s">
-        <v>47</v>
+        <f>J14*L14</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N14" t="s">
+        <v>352</v>
+      </c>
+      <c r="O14" t="str">
+        <f>_xlfn.CONCAT(N14, "-",C14)</f>
+        <v>MBP-F2, F3</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
       <c r="B15" t="s">
-        <v>312</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>263</v>
+        <v>141</v>
       </c>
       <c r="E15" t="s">
-        <v>262</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="G15" t="s">
-        <v>338</v>
-      </c>
-      <c r="H15" t="s">
-        <v>337</v>
-      </c>
-      <c r="J15" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H15), H15)</f>
-        <v>732-12256-1-ND</v>
+        <v>96</v>
+      </c>
+      <c r="I15" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G15), G15)</f>
+        <v>507-1780-1-ND</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
       </c>
       <c r="K15">
         <v>2</v>
       </c>
       <c r="L15" s="3">
-        <v>0.1</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="M15" s="3">
-        <f>K15*L15</f>
-        <v>0.2</v>
+        <f>J15*L15</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N15" t="s">
+        <v>352</v>
+      </c>
+      <c r="O15" t="str">
+        <f>_xlfn.CONCAT(N15, "-",C15)</f>
+        <v>MBP-F1</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>320</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>272</v>
-      </c>
-      <c r="E16" t="s">
-        <v>87</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="E16" s="5"/>
       <c r="F16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" t="s">
-        <v>335</v>
-      </c>
-      <c r="J16" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H16), H16)</f>
-        <v>1276-6471-1-ND</v>
+        <v>106</v>
+      </c>
+      <c r="G16" t="s">
+        <v>347</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G16), G16)</f>
+        <v>2057-PH2-06-UA-ND</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
       </c>
       <c r="K16">
-        <v>4</v>
+        <f>J16</f>
+        <v>1</v>
       </c>
       <c r="L16" s="3">
-        <v>4.7E-2</v>
+        <v>0.12</v>
       </c>
       <c r="M16" s="3">
-        <f>K16*L16</f>
-        <v>0.188</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J16*L16</f>
+        <v>0.12</v>
+      </c>
+      <c r="N16" t="s">
+        <v>351</v>
+      </c>
+      <c r="O16" t="str">
+        <f>_xlfn.CONCAT(N16, "-",C16)</f>
+        <v>PSB-J1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>249</v>
+      </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>320</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>268</v>
+        <v>164</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" t="s">
-        <v>336</v>
-      </c>
-      <c r="J17" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H17), H17)</f>
-        <v>1276-6455-1-ND</v>
+        <v>243</v>
+      </c>
+      <c r="G17" t="s">
+        <v>248</v>
+      </c>
+      <c r="I17" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G17), G17)</f>
+        <v>2057-PH1-06-UA-ND</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>3</v>
+        <f>J17</f>
+        <v>1</v>
       </c>
       <c r="L17" s="3">
-        <v>0.108</v>
+        <v>0.12</v>
       </c>
       <c r="M17" s="3">
-        <f>K17*L17</f>
-        <v>0.32400000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J17*L17</f>
+        <v>0.12</v>
+      </c>
+      <c r="N17" t="s">
+        <v>352</v>
+      </c>
+      <c r="O17" t="str">
+        <f>_xlfn.CONCAT(N17, "-",C17)</f>
+        <v>MBP-J3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>320</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" t="s">
-        <v>296</v>
-      </c>
-      <c r="E18" t="s">
-        <v>102</v>
-      </c>
-      <c r="H18" t="s">
-        <v>65</v>
-      </c>
-      <c r="J18" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H18), H18)</f>
-        <v>576-1048-1-ND</v>
+        <v>346</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" t="s">
+        <v>314</v>
+      </c>
+      <c r="G18" t="s">
+        <v>344</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G18), G18)</f>
+        <v>2057-PH2-12-UA-ND</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <f>J18</f>
+        <v>2</v>
       </c>
       <c r="L18" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.18</v>
       </c>
       <c r="M18" s="3">
-        <f>K18*L18</f>
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="O18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J18*L18</f>
+        <v>0.36</v>
+      </c>
+      <c r="N18" t="s">
+        <v>352</v>
+      </c>
+      <c r="O18" t="str">
+        <f>_xlfn.CONCAT(N18, "-",C18)</f>
+        <v>MBP-J4, J3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>320</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" t="s">
-        <v>293</v>
-      </c>
-      <c r="E19" t="s">
-        <v>145</v>
-      </c>
-      <c r="H19" t="s">
-        <v>69</v>
-      </c>
-      <c r="J19" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H19), H19)</f>
-        <v>LM324DR2GOSCT-ND</v>
+        <v>161</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" t="s">
+        <v>341</v>
+      </c>
+      <c r="G19" t="s">
+        <v>339</v>
+      </c>
+      <c r="I19" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G19), G19)</f>
+        <v>2057-USB-B-S-RA-WT-SPCC-ND</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
       </c>
       <c r="K19">
-        <v>2</v>
+        <f>J19</f>
+        <v>1</v>
       </c>
       <c r="L19" s="3">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="M19" s="3">
-        <f>K19*L19</f>
-        <v>0.7</v>
-      </c>
-      <c r="O19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J19*L19</f>
+        <v>0.45</v>
+      </c>
+      <c r="N19" t="s">
+        <v>352</v>
+      </c>
+      <c r="O19" t="str">
+        <f>_xlfn.CONCAT(N19, "-",C19)</f>
+        <v>MBP-J2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>250</v>
+      </c>
       <c r="B20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" t="s">
-        <v>157</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>320</v>
+      </c>
+      <c r="C20" t="s">
+        <v>258</v>
+      </c>
+      <c r="E20" t="s">
+        <v>243</v>
+      </c>
       <c r="G20" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20" t="s">
-        <v>347</v>
-      </c>
-      <c r="J20" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H20), H20)</f>
-        <v>2057-PH2-06-UA-ND</v>
+        <v>251</v>
+      </c>
+      <c r="I20" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G20), G20)</f>
+        <v>S7039-ND</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
       </c>
       <c r="K20">
+        <f>J20</f>
         <v>1</v>
       </c>
       <c r="L20" s="3">
-        <v>0.12</v>
+        <v>0.53</v>
       </c>
       <c r="M20" s="3">
-        <f>K20*L20</f>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J20*L20</f>
+        <v>0.53</v>
+      </c>
+      <c r="N20" t="s">
+        <v>351</v>
+      </c>
+      <c r="O20" t="str">
+        <f>_xlfn.CONCAT(N20, "-",C20)</f>
+        <v>PSB-J5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>340</v>
+      </c>
       <c r="B21" t="s">
-        <v>340</v>
-      </c>
-      <c r="D21" t="s">
+        <v>320</v>
+      </c>
+      <c r="C21" t="s">
         <v>161</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" t="s">
+        <v>343</v>
+      </c>
       <c r="G21" t="s">
-        <v>343</v>
-      </c>
-      <c r="H21" t="s">
         <v>342</v>
       </c>
-      <c r="J21" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H21), H21)</f>
+      <c r="I21" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G21), G21)</f>
         <v>102-4000-ND</v>
       </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
       <c r="K21">
+        <f>J21</f>
         <v>1</v>
       </c>
       <c r="L21" s="3">
         <v>0.75</v>
       </c>
       <c r="M21" s="3">
-        <f>K21*L21</f>
+        <f>J21*L21</f>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>352</v>
+      </c>
+      <c r="O21" t="str">
+        <f>_xlfn.CONCAT(N21, "-",C21)</f>
+        <v>MBP-J2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>293</v>
       </c>
       <c r="D22" t="s">
-        <v>161</v>
-      </c>
-      <c r="F22" s="5"/>
+        <v>145</v>
+      </c>
       <c r="G22" t="s">
-        <v>341</v>
-      </c>
-      <c r="H22" t="s">
-        <v>339</v>
-      </c>
-      <c r="J22" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H22), H22)</f>
-        <v>2057-USB-B-S-RA-WT-SPCC-ND</v>
+        <v>69</v>
+      </c>
+      <c r="I22" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G22), G22)</f>
+        <v>LM324DR2GOSCT-ND</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <f>J22</f>
+        <v>2</v>
       </c>
       <c r="L22" s="3">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="M22" s="3">
-        <f>K22*L22</f>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J22*L22</f>
+        <v>0.7</v>
+      </c>
+      <c r="N22" t="s">
+        <v>352</v>
+      </c>
+      <c r="O22" t="str">
+        <f>_xlfn.CONCAT(N22, "-",C22)</f>
+        <v>MBP-IC1, IC2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
       <c r="B23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" t="s">
-        <v>346</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>223</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>72</v>
+      </c>
       <c r="G23" t="s">
-        <v>314</v>
-      </c>
-      <c r="H23" t="s">
-        <v>344</v>
-      </c>
-      <c r="J23" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H23), H23)</f>
-        <v>2057-PH2-12-UA-ND</v>
+        <v>71</v>
+      </c>
+      <c r="I23" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G23), G23)</f>
+        <v>AZ1117IH-5.0TRG1DICT-ND</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
       </c>
       <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="M23" s="3">
+        <f>J23*L23</f>
+        <v>0.36</v>
+      </c>
+      <c r="N23" t="s">
+        <v>352</v>
+      </c>
+      <c r="O23" t="str">
+        <f>_xlfn.CONCAT(N23, "-",C23)</f>
+        <v>MBP-U2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>286</v>
+      </c>
+      <c r="D24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" t="s">
+        <v>115</v>
+      </c>
+      <c r="I24" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G24), G24)</f>
+        <v>497-1192-1-ND</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f>J24</f>
+        <v>1</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="M24" s="3">
+        <f>J24*L24</f>
+        <v>0.4</v>
+      </c>
+      <c r="N24" t="s">
+        <v>352</v>
+      </c>
+      <c r="O24" t="str">
+        <f>_xlfn.CONCAT(N24, "-",C24)</f>
+        <v>MBP-U6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>247</v>
+      </c>
+      <c r="D25" t="s">
+        <v>316</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="G25" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="I25" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G25), G25)</f>
+        <v>TLP185(GB-TPLSECT-ND</v>
+      </c>
+      <c r="J25">
         <v>2</v>
       </c>
-      <c r="L23" s="3">
-        <v>0.18</v>
-      </c>
-      <c r="M23" s="3">
-        <f>K23*L23</f>
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>250</v>
-      </c>
-      <c r="D24" t="s">
-        <v>258</v>
-      </c>
-      <c r="F24" t="s">
-        <v>243</v>
-      </c>
-      <c r="H24" t="s">
-        <v>251</v>
-      </c>
-      <c r="J24" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H24), H24)</f>
-        <v>S7039-ND</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24" s="3">
-        <v>0.53</v>
-      </c>
-      <c r="M24" s="3">
-        <f>K24*L24</f>
-        <v>0.53</v>
-      </c>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" t="s">
-        <v>247</v>
-      </c>
-      <c r="E25" t="s">
-        <v>316</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="H25" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="J25" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H25), H25)</f>
-        <v>TLP185(GB-TPLSECT-ND</v>
-      </c>
       <c r="K25">
+        <f>J25</f>
         <v>2</v>
       </c>
       <c r="L25" s="3">
         <v>0.42</v>
       </c>
       <c r="M25" s="3">
-        <f>K25*L25</f>
+        <f>J25*L25</f>
         <v>0.84</v>
       </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>351</v>
+      </c>
+      <c r="O25" t="str">
+        <f>_xlfn.CONCAT(N25, "-",C25)</f>
+        <v>PSB-NA</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="F26" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" t="s">
-        <v>98</v>
-      </c>
-      <c r="H26" t="s">
-        <v>77</v>
-      </c>
-      <c r="J26" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H26), H26)</f>
-        <v>887-2015-ND</v>
+        <v>355</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G26), G26)</f>
+        <v>336-5888-1-ND</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
       </c>
       <c r="K26">
+        <f>J26</f>
         <v>1</v>
       </c>
       <c r="L26" s="3">
-        <v>0.3</v>
+        <v>1.35</v>
       </c>
       <c r="M26" s="3">
-        <f>K26*L26</f>
-        <v>0.3</v>
-      </c>
-      <c r="O26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J26*L26</f>
+        <v>1.35</v>
+      </c>
+      <c r="N26" t="s">
+        <v>351</v>
+      </c>
+      <c r="O26" t="str">
+        <f>_xlfn.CONCAT(N26, "-",C26)</f>
+        <v>PSB-U3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
+        <v>220</v>
+      </c>
+      <c r="E27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G27), G27)</f>
+        <v>ATMEGA328PB-AURCT-ND</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <f>J27</f>
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>1.42</v>
+      </c>
+      <c r="M27" s="3">
+        <f>J27*L27</f>
+        <v>1.42</v>
+      </c>
+      <c r="N27" t="s">
+        <v>351</v>
+      </c>
+      <c r="O27" t="str">
+        <f>_xlfn.CONCAT(N27, "-",C27)</f>
+        <v>PSB-U1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>226</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G28), G28)</f>
+        <v>AP2114HA-3.3TRG1DICT-ND</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>3</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="M28" s="3">
+        <f>J28*L28</f>
+        <v>0.36</v>
+      </c>
+      <c r="N28" t="s">
+        <v>352</v>
+      </c>
+      <c r="O28" t="str">
+        <f>_xlfn.CONCAT(N28, "-",C28)</f>
+        <v>MBP-U3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" t="s">
         <v>35</v>
       </c>
-      <c r="D27" t="s">
-        <v>271</v>
-      </c>
-      <c r="E27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="C29" t="s">
+        <v>265</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
         <v>100</v>
       </c>
-      <c r="G27" t="s">
-        <v>330</v>
-      </c>
-      <c r="H27" t="s">
-        <v>327</v>
-      </c>
-      <c r="J27" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H27), H27)</f>
-        <v>RMCF0805FT1K00CT-ND</v>
-      </c>
-      <c r="K27">
-        <v>4</v>
-      </c>
-      <c r="L27" s="3">
-        <v>2.7E-2</v>
-      </c>
-      <c r="M27" s="3">
-        <f>K27*L27</f>
-        <v>0.108</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" t="s">
-        <v>265</v>
-      </c>
-      <c r="E28">
+      <c r="F29" t="s">
+        <v>332</v>
+      </c>
+      <c r="G29" t="s">
+        <v>331</v>
+      </c>
+      <c r="I29" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G29), G29)</f>
+        <v>CR0805-JW-100ELFCT-ND</v>
+      </c>
+      <c r="J29">
+        <v>8</v>
+      </c>
+      <c r="K29">
         <v>10</v>
-      </c>
-      <c r="F28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G28" t="s">
-        <v>332</v>
-      </c>
-      <c r="H28" t="s">
-        <v>331</v>
-      </c>
-      <c r="J28" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H28), H28)</f>
-        <v>CR0805-JW-100ELFCT-ND</v>
-      </c>
-      <c r="K28">
-        <v>8</v>
-      </c>
-      <c r="L28" s="3">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M28" s="3">
-        <f>K28*L28</f>
-        <v>0.14399999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>313</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" t="s">
-        <v>281</v>
-      </c>
-      <c r="E29" t="s">
-        <v>280</v>
-      </c>
-      <c r="F29" t="s">
-        <v>100</v>
-      </c>
-      <c r="G29" t="s">
-        <v>329</v>
-      </c>
-      <c r="H29" t="s">
-        <v>328</v>
-      </c>
-      <c r="J29" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H29), H29)</f>
-        <v>CR0805-JW-472ELFCT-ND</v>
-      </c>
-      <c r="K29">
-        <v>2</v>
       </c>
       <c r="L29" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="M29" s="3">
-        <f>K29*L29</f>
+        <f>J29*L29</f>
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="N29" t="s">
+        <v>352</v>
+      </c>
+      <c r="O29" t="str">
+        <f>_xlfn.CONCAT(N29, "-",C29)</f>
+        <v>MBP-R29, R30, R31, R32, R33, R34, R35, R36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>313</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>281</v>
+      </c>
+      <c r="D30" t="s">
+        <v>280</v>
+      </c>
+      <c r="E30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" t="s">
+        <v>329</v>
+      </c>
+      <c r="G30" t="s">
+        <v>328</v>
+      </c>
+      <c r="I30" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G30), G30)</f>
+        <v>CR0805-JW-472ELFCT-ND</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <v>10</v>
+      </c>
+      <c r="L30" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M30" s="3">
+        <f>J30*L30</f>
         <v>3.5999999999999997E-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="N30" t="s">
+        <v>352</v>
+      </c>
+      <c r="O30" t="str">
+        <f>_xlfn.CONCAT(N30, "-",C30)</f>
+        <v>MBP-R3, R4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" t="s">
         <v>35</v>
       </c>
-      <c r="D30" t="s">
-        <v>279</v>
-      </c>
-      <c r="E30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="C31" t="s">
+        <v>271</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" t="s">
         <v>100</v>
       </c>
-      <c r="G30" t="s">
-        <v>322</v>
-      </c>
-      <c r="H30" t="s">
-        <v>321</v>
-      </c>
-      <c r="J30" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H30), H30)</f>
-        <v>RMCF0805FT30K1CT-ND</v>
-      </c>
-      <c r="K30">
-        <v>8</v>
-      </c>
-      <c r="L30" s="3">
-        <v>2.7E-2</v>
-      </c>
-      <c r="M30" s="3">
-        <f>K30*L30</f>
-        <v>0.216</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" t="s">
-        <v>267</v>
-      </c>
-      <c r="E31" t="s">
-        <v>80</v>
-      </c>
       <c r="F31" t="s">
-        <v>100</v>
+        <v>330</v>
       </c>
       <c r="G31" t="s">
-        <v>324</v>
-      </c>
-      <c r="H31" t="s">
-        <v>323</v>
-      </c>
-      <c r="J31" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H31), H31)</f>
-        <v>RMCF0805FT10K0CT-ND</v>
+        <v>327</v>
+      </c>
+      <c r="I31" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G31), G31)</f>
+        <v>RMCF0805FT1K00CT-ND</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
       </c>
       <c r="K31">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="L31" s="3">
         <v>2.7E-2</v>
       </c>
       <c r="M31" s="3">
-        <f>K31*L31</f>
-        <v>0.378</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J31*L31</f>
+        <v>0.108</v>
+      </c>
+      <c r="N31" t="s">
+        <v>352</v>
+      </c>
+      <c r="O31" t="str">
+        <f>_xlfn.CONCAT(N31, "-",C31)</f>
+        <v>MBP-R1, R2, R21, R22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>279</v>
       </c>
       <c r="D32" t="s">
-        <v>270</v>
+        <v>81</v>
       </c>
       <c r="E32" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="F32" t="s">
-        <v>100</v>
+        <v>322</v>
       </c>
       <c r="G32" t="s">
-        <v>325</v>
-      </c>
-      <c r="H32" t="s">
-        <v>326</v>
-      </c>
-      <c r="J32" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H32), H32)</f>
-        <v>RMCF0805FT15K0CT-ND</v>
+        <v>321</v>
+      </c>
+      <c r="I32" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G32), G32)</f>
+        <v>RMCF0805FT30K1CT-ND</v>
+      </c>
+      <c r="J32">
+        <v>8</v>
       </c>
       <c r="K32">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L32" s="3">
         <v>2.7E-2</v>
       </c>
       <c r="M32" s="3">
-        <f>K32*L32</f>
+        <f>J32*L32</f>
+        <v>0.216</v>
+      </c>
+      <c r="N32" t="s">
+        <v>351</v>
+      </c>
+      <c r="O32" t="str">
+        <f>_xlfn.CONCAT(N32, "-",C32)</f>
+        <v>PSB-R5, R7, R11, R14, R15, R18, R19, R26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>267</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" t="s">
+        <v>324</v>
+      </c>
+      <c r="G33" t="s">
+        <v>323</v>
+      </c>
+      <c r="I33" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G33), G33)</f>
+        <v>RMCF0805FT10K0CT-ND</v>
+      </c>
+      <c r="J33">
+        <v>14</v>
+      </c>
+      <c r="K33">
+        <v>100</v>
+      </c>
+      <c r="L33" s="3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="M33" s="3">
+        <f>J33*L33</f>
+        <v>0.378</v>
+      </c>
+      <c r="N33" t="s">
+        <v>352</v>
+      </c>
+      <c r="O33" t="str">
+        <f>_xlfn.CONCAT(N33, "-",C33)</f>
+        <v>MBP-R6, R8, R10, R12, R13, R16, R17, R20, R24, R25, R27, R28, R37, R38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>270</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" t="s">
+        <v>325</v>
+      </c>
+      <c r="G34" t="s">
+        <v>326</v>
+      </c>
+      <c r="I34" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G34), G34)</f>
+        <v>RMCF0805FT15K0CT-ND</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
+        <v>10</v>
+      </c>
+      <c r="L34" s="3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="M34" s="3">
+        <f>J34*L34</f>
         <v>5.3999999999999999E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" t="s">
-        <v>304</v>
-      </c>
-      <c r="F33" t="s">
-        <v>109</v>
-      </c>
-      <c r="G33" t="s">
-        <v>108</v>
-      </c>
-      <c r="H33" t="s">
-        <v>107</v>
-      </c>
-      <c r="J33" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H33), H33)</f>
-        <v>CKN12220-1-ND</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33" s="3">
+      <c r="N34" t="s">
+        <v>352</v>
+      </c>
+      <c r="O34" t="str">
+        <f>_xlfn.CONCAT(N34, "-",C34)</f>
+        <v>MBP-R9, R23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>244</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" t="s">
+        <v>240</v>
+      </c>
+      <c r="G35" t="s">
+        <v>239</v>
+      </c>
+      <c r="I35" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G35), G35)</f>
+        <v>RMCF1206JT1K20CT-ND</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35" s="3">
         <v>0.1</v>
       </c>
-      <c r="M33" s="3">
-        <f>K33*L33</f>
+      <c r="M35" s="3">
+        <f>J35*L35</f>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" t="s">
-        <v>220</v>
-      </c>
-      <c r="F34" t="s">
-        <v>97</v>
-      </c>
-      <c r="H34" t="s">
-        <v>85</v>
-      </c>
-      <c r="I34" t="s">
-        <v>63</v>
-      </c>
-      <c r="J34" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H34), H34)</f>
-        <v>ATMEGA328PB-AURCT-ND</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34" s="3">
-        <v>1.42</v>
-      </c>
-      <c r="M34" s="3">
-        <f>K34*L34</f>
-        <v>1.42</v>
-      </c>
-      <c r="O34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" t="s">
-        <v>223</v>
-      </c>
-      <c r="F35" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" t="s">
-        <v>72</v>
-      </c>
-      <c r="H35" t="s">
-        <v>71</v>
-      </c>
-      <c r="J35" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H35), H35)</f>
-        <v>AZ1117IH-5.0TRG1DICT-ND</v>
-      </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
-      <c r="L35" s="3">
-        <v>0.36</v>
-      </c>
-      <c r="M35" s="3">
-        <f>K35*L35</f>
-        <v>0.36</v>
-      </c>
-      <c r="O35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>351</v>
+      </c>
+      <c r="O35" t="str">
+        <f>_xlfn.CONCAT(N35, "-",C35)</f>
+        <v>PSB-R31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>245</v>
       </c>
       <c r="D36" t="s">
-        <v>226</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J36" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H36), H36)</f>
-        <v>336-5888-1-ND</v>
+        <v>44</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" t="s">
+        <v>238</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="I36" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G36), G36)</f>
+        <v>RMCF1206JT390RCT-ND</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
       </c>
       <c r="K36">
         <v>1</v>
       </c>
       <c r="L36" s="3">
-        <v>1.35</v>
+        <v>0.1</v>
       </c>
       <c r="M36" s="3">
-        <f>K36*L36</f>
-        <v>1.35</v>
-      </c>
-      <c r="O36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J36*L36</f>
+        <v>0.1</v>
+      </c>
+      <c r="N36" t="s">
+        <v>352</v>
+      </c>
+      <c r="O36" t="str">
+        <f>_xlfn.CONCAT(N36, "-",C36)</f>
+        <v>MBP-R32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>246</v>
       </c>
       <c r="D37" t="s">
-        <v>308</v>
-      </c>
-      <c r="H37" t="s">
-        <v>75</v>
-      </c>
-      <c r="J37" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H37), H37)</f>
-        <v>1727-1582-1-ND</v>
+        <v>43</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" t="s">
+        <v>236</v>
+      </c>
+      <c r="G37" t="s">
+        <v>235</v>
+      </c>
+      <c r="I37" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G37), G37)</f>
+        <v>RMCF1206JT150RCT-ND</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
       </c>
       <c r="K37">
-        <v>4</v>
+        <f>J37</f>
+        <v>1</v>
       </c>
       <c r="L37" s="3">
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="M37" s="3">
-        <f>K37*L37</f>
-        <v>1.24</v>
-      </c>
-      <c r="O37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J37*L37</f>
+        <v>0.1</v>
+      </c>
+      <c r="N37" t="s">
+        <v>352</v>
+      </c>
+      <c r="O37" t="str">
+        <f>_xlfn.CONCAT(N37, "-",C37)</f>
+        <v>MBP-R33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>234</v>
+      </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>319</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" t="s">
-        <v>286</v>
-      </c>
-      <c r="E38" t="s">
-        <v>112</v>
+        <v>241</v>
+      </c>
+      <c r="F38" t="s">
+        <v>318</v>
       </c>
       <c r="G38" t="s">
-        <v>114</v>
-      </c>
-      <c r="H38" t="s">
-        <v>113</v>
-      </c>
-      <c r="I38" t="s">
-        <v>115</v>
-      </c>
-      <c r="J38" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",H38), H38)</f>
-        <v>497-1192-1-ND</v>
+        <v>317</v>
+      </c>
+      <c r="I38" s="11" t="str">
+        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G38), G38)</f>
+        <v>401-2001-ND</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
       </c>
       <c r="K38">
+        <f>J38</f>
         <v>1</v>
       </c>
       <c r="L38" s="3">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="M38" s="3">
-        <f>K38*L38</f>
-        <v>0.4</v>
-      </c>
-      <c r="O38" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+        <f>J38*L38</f>
+        <v>0.43</v>
+      </c>
+      <c r="N38" t="s">
+        <v>352</v>
+      </c>
+      <c r="O38" t="str">
+        <f>_xlfn.CONCAT(N38, "-",C38)</f>
+        <v>MBP-S3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L41" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="M41" s="6">
+        <f>SUM(M2:M40)</f>
+        <v>19.465999999999994</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M45" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:O32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="O2:O38">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="unchecked">
-      <formula>NOT(ISERROR(SEARCH("unchecked",O2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Need">
-      <formula>NOT(ISERROR(SEARCH("Need",O2)))</formula>
+  <autoFilter ref="A1:M32" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M38">
+      <sortCondition ref="B1:B32"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O40">
+    <sortCondition ref="C2:C40"/>
+  </sortState>
+  <conditionalFormatting sqref="K2:K38">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>IF(K2 &lt;&gt; J2, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="O2:O38" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"Built-In,Imported Unchecked,Built-In Unchecked,Custom,Custom-Unchecked,Needs Model"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3762,10 +4120,10 @@
   </sheetData>
   <autoFilter ref="B1:O34" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="O2:O33">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="unchecked">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="unchecked">
       <formula>NOT(ISERROR(SEARCH("unchecked",O2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Need">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Need">
       <formula>NOT(ISERROR(SEARCH("Need",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3783,7 +4141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -3867,7 +4225,7 @@
         <v>333</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G2), G2)</f>
+        <f t="shared" ref="I2:I34" si="0">HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G2), G2)</f>
         <v>732-7816-1-ND</v>
       </c>
       <c r="J2">
@@ -3877,7 +4235,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="L2" s="3">
-        <f>J2*K2</f>
+        <f t="shared" ref="L2:L34" si="1">J2*K2</f>
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="N2" t="s">
@@ -3907,7 +4265,7 @@
         <v>337</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
+        <f t="shared" si="0"/>
         <v>732-12256-1-ND</v>
       </c>
       <c r="J3">
@@ -3917,7 +4275,7 @@
         <v>0.1</v>
       </c>
       <c r="L3" s="3">
-        <f>J3*K3</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
     </row>
@@ -3941,7 +4299,7 @@
         <v>335</v>
       </c>
       <c r="I4" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G4), G4)</f>
+        <f t="shared" si="0"/>
         <v>1276-6471-1-ND</v>
       </c>
       <c r="J4">
@@ -3951,7 +4309,7 @@
         <v>4.7E-2</v>
       </c>
       <c r="L4" s="3">
-        <f>J4*K4</f>
+        <f t="shared" si="1"/>
         <v>0.188</v>
       </c>
     </row>
@@ -3975,7 +4333,7 @@
         <v>336</v>
       </c>
       <c r="I5" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G5), G5)</f>
+        <f t="shared" si="0"/>
         <v>1276-6455-1-ND</v>
       </c>
       <c r="J5">
@@ -3985,7 +4343,7 @@
         <v>0.108</v>
       </c>
       <c r="L5" s="3">
-        <f>J5*K5</f>
+        <f t="shared" si="1"/>
         <v>0.32400000000000001</v>
       </c>
     </row>
@@ -4006,7 +4364,7 @@
         <v>65</v>
       </c>
       <c r="I6" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G6), G6)</f>
+        <f t="shared" si="0"/>
         <v>576-1048-1-ND</v>
       </c>
       <c r="J6">
@@ -4016,7 +4374,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="L6" s="3">
-        <f>J6*K6</f>
+        <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="N6" t="s">
@@ -4040,7 +4398,7 @@
         <v>69</v>
       </c>
       <c r="I7" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G7), G7)</f>
+        <f t="shared" si="0"/>
         <v>LM324DR2GOSCT-ND</v>
       </c>
       <c r="J7">
@@ -4050,7 +4408,7 @@
         <v>0.35</v>
       </c>
       <c r="L7" s="3">
-        <f>J7*K7</f>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="N7" t="s">
@@ -4072,7 +4430,7 @@
         <v>347</v>
       </c>
       <c r="I8" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G8), G8)</f>
+        <f t="shared" si="0"/>
         <v>2057-PH2-06-UA-ND</v>
       </c>
       <c r="J8">
@@ -4082,7 +4440,7 @@
         <v>0.12</v>
       </c>
       <c r="L8" s="3">
-        <f>J8*K8</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
     </row>
@@ -4101,7 +4459,7 @@
         <v>342</v>
       </c>
       <c r="I9" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G9), G9)</f>
+        <f t="shared" si="0"/>
         <v>102-4000-ND</v>
       </c>
       <c r="J9">
@@ -4111,7 +4469,7 @@
         <v>0.75</v>
       </c>
       <c r="L9" s="3">
-        <f>J9*K9</f>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
     </row>
@@ -4130,7 +4488,7 @@
         <v>339</v>
       </c>
       <c r="I10" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G10), G10)</f>
+        <f t="shared" si="0"/>
         <v>2057-USB-B-S-RA-WT-SPCC-ND</v>
       </c>
       <c r="J10">
@@ -4140,7 +4498,7 @@
         <v>0.45</v>
       </c>
       <c r="L10" s="3">
-        <f>J10*K10</f>
+        <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
     </row>
@@ -4158,7 +4516,7 @@
         <v>344</v>
       </c>
       <c r="I11" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G11), G11)</f>
+        <f t="shared" si="0"/>
         <v>2057-PH2-12-UA-ND</v>
       </c>
       <c r="J11">
@@ -4168,7 +4526,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="3">
-        <f>J11*K11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N11" s="4"/>
@@ -4188,7 +4546,7 @@
         <v>344</v>
       </c>
       <c r="I12" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G12), G12)</f>
+        <f t="shared" si="0"/>
         <v>2057-PH2-12-UA-ND</v>
       </c>
       <c r="J12">
@@ -4198,7 +4556,7 @@
         <v>0.18</v>
       </c>
       <c r="L12" s="3">
-        <f>J12*K12</f>
+        <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
     </row>
@@ -4216,7 +4574,7 @@
         <v>251</v>
       </c>
       <c r="I13" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G13), G13)</f>
+        <f t="shared" si="0"/>
         <v>S7039-ND</v>
       </c>
       <c r="J13">
@@ -4226,7 +4584,7 @@
         <v>0.53</v>
       </c>
       <c r="L13" s="3">
-        <f>J13*K13</f>
+        <f t="shared" si="1"/>
         <v>0.53</v>
       </c>
       <c r="N13" s="4"/>
@@ -4249,7 +4607,7 @@
         <v>315</v>
       </c>
       <c r="I14" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G14), G14)</f>
+        <f t="shared" si="0"/>
         <v>TLP185(GB-TPLSECT-ND</v>
       </c>
       <c r="J14">
@@ -4259,7 +4617,7 @@
         <v>0.42</v>
       </c>
       <c r="L14" s="3">
-        <f>J14*K14</f>
+        <f t="shared" si="1"/>
         <v>0.84</v>
       </c>
     </row>
@@ -4283,7 +4641,7 @@
         <v>77</v>
       </c>
       <c r="I15" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G15), G15)</f>
+        <f t="shared" si="0"/>
         <v>887-2015-ND</v>
       </c>
       <c r="J15">
@@ -4293,7 +4651,7 @@
         <v>0.3</v>
       </c>
       <c r="L15" s="3">
-        <f>J15*K15</f>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="N15" t="s">
@@ -4323,7 +4681,7 @@
         <v>327</v>
       </c>
       <c r="I16" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G16), G16)</f>
+        <f t="shared" si="0"/>
         <v>RMCF0805FT1K00CT-ND</v>
       </c>
       <c r="J16">
@@ -4333,7 +4691,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="L16" s="3">
-        <f>J16*K16</f>
+        <f t="shared" si="1"/>
         <v>0.108</v>
       </c>
     </row>
@@ -4360,7 +4718,7 @@
         <v>331</v>
       </c>
       <c r="I17" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G17), G17)</f>
+        <f t="shared" si="0"/>
         <v>CR0805-JW-100ELFCT-ND</v>
       </c>
       <c r="J17">
@@ -4370,7 +4728,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="L17" s="3">
-        <f>J17*K17</f>
+        <f t="shared" si="1"/>
         <v>0.14399999999999999</v>
       </c>
     </row>
@@ -4397,7 +4755,7 @@
         <v>328</v>
       </c>
       <c r="I18" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G18), G18)</f>
+        <f t="shared" si="0"/>
         <v>CR0805-JW-472ELFCT-ND</v>
       </c>
       <c r="J18">
@@ -4407,7 +4765,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="L18" s="3">
-        <f>J18*K18</f>
+        <f t="shared" si="1"/>
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
@@ -4434,7 +4792,7 @@
         <v>321</v>
       </c>
       <c r="I19" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G19), G19)</f>
+        <f t="shared" si="0"/>
         <v>RMCF0805FT30K1CT-ND</v>
       </c>
       <c r="J19">
@@ -4444,7 +4802,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="L19" s="3">
-        <f>J19*K19</f>
+        <f t="shared" si="1"/>
         <v>0.216</v>
       </c>
     </row>
@@ -4471,7 +4829,7 @@
         <v>323</v>
       </c>
       <c r="I20" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G20), G20)</f>
+        <f t="shared" si="0"/>
         <v>RMCF0805FT10K0CT-ND</v>
       </c>
       <c r="J20">
@@ -4481,7 +4839,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="L20" s="3">
-        <f>J20*K20</f>
+        <f t="shared" si="1"/>
         <v>0.378</v>
       </c>
     </row>
@@ -4508,7 +4866,7 @@
         <v>326</v>
       </c>
       <c r="I21" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G21), G21)</f>
+        <f t="shared" si="0"/>
         <v>RMCF0805FT15K0CT-ND</v>
       </c>
       <c r="J21">
@@ -4518,7 +4876,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="L21" s="3">
-        <f>J21*K21</f>
+        <f t="shared" si="1"/>
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
@@ -4542,7 +4900,7 @@
         <v>107</v>
       </c>
       <c r="I22" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G22), G22)</f>
+        <f t="shared" si="0"/>
         <v>CKN12220-1-ND</v>
       </c>
       <c r="J22">
@@ -4552,7 +4910,7 @@
         <v>0.1</v>
       </c>
       <c r="L22" s="3">
-        <f>J22*K22</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
     </row>
@@ -4576,7 +4934,7 @@
         <v>63</v>
       </c>
       <c r="I23" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G23), G23)</f>
+        <f t="shared" si="0"/>
         <v>ATMEGA328PB-AURCT-ND</v>
       </c>
       <c r="J23">
@@ -4586,7 +4944,7 @@
         <v>1.42</v>
       </c>
       <c r="L23" s="3">
-        <f>J23*K23</f>
+        <f t="shared" si="1"/>
         <v>1.42</v>
       </c>
       <c r="N23" t="s">
@@ -4616,7 +4974,7 @@
         <v>71</v>
       </c>
       <c r="I24" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G24), G24)</f>
+        <f t="shared" si="0"/>
         <v>AZ1117IH-5.0TRG1DICT-ND</v>
       </c>
       <c r="J24">
@@ -4626,7 +4984,7 @@
         <v>0.36</v>
       </c>
       <c r="L24" s="3">
-        <f>J24*K24</f>
+        <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
       <c r="N24" t="s">
@@ -4647,7 +5005,7 @@
         <v>74</v>
       </c>
       <c r="I25" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G25), G25)</f>
+        <f t="shared" si="0"/>
         <v>336-5888-1-ND</v>
       </c>
       <c r="J25">
@@ -4657,7 +5015,7 @@
         <v>1.35</v>
       </c>
       <c r="L25" s="3">
-        <f>J25*K25</f>
+        <f t="shared" si="1"/>
         <v>1.35</v>
       </c>
       <c r="N25" t="s">
@@ -4678,7 +5036,7 @@
         <v>75</v>
       </c>
       <c r="I26" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G26), G26)</f>
+        <f t="shared" si="0"/>
         <v>1727-1582-1-ND</v>
       </c>
       <c r="J26">
@@ -4688,7 +5046,7 @@
         <v>0.31</v>
       </c>
       <c r="L26" s="3">
-        <f>J26*K26</f>
+        <f t="shared" si="1"/>
         <v>1.24</v>
       </c>
       <c r="N26" t="s">
@@ -4712,7 +5070,7 @@
         <v>68</v>
       </c>
       <c r="I27" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G27), G27)</f>
+        <f t="shared" si="0"/>
         <v>MCP4728-E/UN-ND</v>
       </c>
       <c r="J27">
@@ -4722,7 +5080,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="3">
-        <f>J27*K27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N27" t="s">
@@ -4752,7 +5110,7 @@
         <v>115</v>
       </c>
       <c r="I28" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G28), G28)</f>
+        <f t="shared" si="0"/>
         <v>497-1192-1-ND</v>
       </c>
       <c r="J28">
@@ -4762,7 +5120,7 @@
         <v>0.4</v>
       </c>
       <c r="L28" s="3">
-        <f>J28*K28</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="N28" t="s">
@@ -4771,68 +5129,68 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I29" s="2">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G29), G29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3">
-        <f>J29*K29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I30" s="2">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G30), G30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3">
-        <f>J30*K30</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I31" s="2">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G31), G31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="3">
-        <f>J31*K31</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I32" s="2">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G32), G32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="3">
-        <f>J32*K32</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I33" s="2">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G33), G33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3">
-        <f>J33*K33</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I34" s="2">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G34), G34)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K34" s="3"/>
       <c r="L34" s="3">
-        <f>J34*K34</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4907,10 +5265,10 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="N2:N34">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="unchecked">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="unchecked">
       <formula>NOT(ISERROR(SEARCH("unchecked",N2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Need">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Need">
       <formula>NOT(ISERROR(SEARCH("Need",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6227,7 +6585,7 @@
     <sortCondition ref="F2:F35"/>
   </sortState>
   <conditionalFormatting sqref="A2:A35">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="extra">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="extra">
       <formula>NOT(ISERROR(SEARCH("extra",A2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Hopefully fixed MBP/PSB mixup
</commit_message>
<xml_diff>
--- a/BOM_Initial.xlsx
+++ b/BOM_Initial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Gilliland\Desktop\All Projects\benchBuddy\benchBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81498D47-0930-42C0-8219-FD00EBEA5D47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA69B12-1671-4263-9A58-042C8A388924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Main Board Additions'!$B$1:$O$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'MCU Board'!$A$1:$N$35</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PurchaseBOM!$A$1:$M$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PurchaseBOM!$A$1:$O$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="360">
   <si>
     <t>Usage</t>
   </si>
@@ -1108,6 +1108,18 @@
   </si>
   <si>
     <t>CP2102N-A02-GQFN24R</t>
+  </si>
+  <si>
+    <t>Passive, Capacitor</t>
+  </si>
+  <si>
+    <t>Passive, Resistor</t>
+  </si>
+  <si>
+    <t>IC, DCDC Converter</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1535,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,93 +1659,96 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>356</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>273</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
         <v>51</v>
       </c>
+      <c r="F3" t="s">
+        <v>334</v>
+      </c>
       <c r="G3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="11" t="str">
+        <v>333</v>
+      </c>
+      <c r="I3" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
-        <v>1276-1007-1-ND</v>
+        <v>732-7816-1-ND</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3">
         <v>10</v>
       </c>
       <c r="L3" s="3">
-        <v>0.04</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="M3" s="3">
         <f>J3*L3</f>
-        <v>0.12</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="N3" t="s">
         <v>352</v>
       </c>
       <c r="O3" t="str">
         <f>_xlfn.CONCAT(N3, "-",C3)</f>
-        <v>MBP-C8, C11, C13</v>
+        <v>MBP-C1, C2</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>312</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>356</v>
       </c>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>262</v>
       </c>
       <c r="E4" t="s">
         <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="G4" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="I4" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G4), G4)</f>
-        <v>732-7816-1-ND</v>
+        <v>732-12256-1-ND</v>
       </c>
       <c r="J4">
         <v>2</v>
       </c>
       <c r="K4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L4" s="3">
-        <v>4.2999999999999997E-2</v>
+        <v>0.1</v>
       </c>
       <c r="M4" s="3">
         <f>J4*L4</f>
-        <v>8.5999999999999993E-2</v>
+        <v>0.2</v>
       </c>
       <c r="N4" t="s">
         <v>352</v>
       </c>
       <c r="O4" t="str">
         <f>_xlfn.CONCAT(N4, "-",C4)</f>
-        <v>MBP-C1, C2</v>
+        <v>MBP-C10, C11</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1741,7 +1756,7 @@
         <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>356</v>
       </c>
       <c r="C5" t="s">
         <v>272</v>
@@ -1782,73 +1797,70 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>312</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>356</v>
       </c>
       <c r="C6" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="D6" t="s">
-        <v>262</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
         <v>51</v>
       </c>
-      <c r="F6" t="s">
-        <v>338</v>
-      </c>
       <c r="G6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I6" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G6), G6)</f>
-        <v>732-12256-1-ND</v>
+        <v>1276-6455-1-ND</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L6" s="3">
-        <v>0.1</v>
+        <v>0.108</v>
       </c>
       <c r="M6" s="3">
         <f>J6*L6</f>
-        <v>0.2</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="N6" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="O6" t="str">
         <f>_xlfn.CONCAT(N6, "-",C6)</f>
-        <v>PSB-C10, C11</v>
+        <v>MBP-C4, C6, C8</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>356</v>
       </c>
       <c r="C7" t="s">
-        <v>268</v>
+        <v>132</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>336</v>
-      </c>
-      <c r="I7" s="2" t="str">
+        <v>59</v>
+      </c>
+      <c r="I7" s="11" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G7), G7)</f>
-        <v>1276-6455-1-ND</v>
+        <v>1276-1007-1-ND</v>
       </c>
       <c r="J7">
         <v>3</v>
@@ -1857,18 +1869,18 @@
         <v>10</v>
       </c>
       <c r="L7" s="3">
-        <v>0.108</v>
+        <v>0.04</v>
       </c>
       <c r="M7" s="3">
         <f>J7*L7</f>
-        <v>0.32400000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="N7" t="s">
         <v>351</v>
       </c>
       <c r="O7" t="str">
         <f>_xlfn.CONCAT(N7, "-",C7)</f>
-        <v>PSB-C4, C6, C8</v>
+        <v>PSB-C8, C11, C13</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1876,7 +1888,7 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>356</v>
       </c>
       <c r="C8" t="s">
         <v>133</v>
@@ -1908,11 +1920,11 @@
         <v>0.432</v>
       </c>
       <c r="N8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O8" t="str">
         <f>_xlfn.CONCAT(N8, "-",C8)</f>
-        <v>MBP-C9, C10, C12, C14</v>
+        <v>PSB-C9, C10, C12, C14</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1953,11 +1965,11 @@
         <v>0.3</v>
       </c>
       <c r="N9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="O9" t="str">
         <f>_xlfn.CONCAT(N9, "-",C9)</f>
-        <v>PSB-Q1</v>
+        <v>MBP-Q1</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1965,7 +1977,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>28</v>
+        <v>358</v>
       </c>
       <c r="C10" t="s">
         <v>179</v>
@@ -2040,11 +2052,11 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="N11" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="O11" t="str">
         <f>_xlfn.CONCAT(N11, "-",C11)</f>
-        <v>PSB-D1</v>
+        <v>MBP-D1</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2087,51 +2099,51 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
         <v>53</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="I13" s="11" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G13), G13)</f>
-        <v>507-1761-1-ND</v>
+        <v>507-1780-1-ND</v>
       </c>
       <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
         <v>2</v>
       </c>
-      <c r="K13">
-        <v>3</v>
-      </c>
       <c r="L13" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="M13" s="3">
         <f>J13*L13</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="N13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O13" t="str">
         <f>_xlfn.CONCAT(N13, "-",C13)</f>
-        <v>MBP-F2, F3</v>
+        <v>PSB-F1</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -2143,14 +2155,14 @@
         <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I14" s="11" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G14), G14)</f>
-        <v>507-1763-1-ND</v>
+        <v>507-1761-1-ND</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -2166,55 +2178,55 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="N14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O14" t="str">
         <f>_xlfn.CONCAT(N14, "-",C14)</f>
-        <v>MBP-F2, F3</v>
+        <v>PSB-F2, F3</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E15" t="s">
         <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="I15" s="11" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G15), G15)</f>
-        <v>507-1780-1-ND</v>
+        <v>507-1763-1-ND</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L15" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M15" s="3">
         <f>J15*L15</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="N15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O15" t="str">
         <f>_xlfn.CONCAT(N15, "-",C15)</f>
-        <v>MBP-F1</v>
+        <v>PSB-F2, F3</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2253,32 +2265,33 @@
         <v>0.12</v>
       </c>
       <c r="N16" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="O16" t="str">
         <f>_xlfn.CONCAT(N16, "-",C16)</f>
-        <v>PSB-J1</v>
+        <v>MBP-J1</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>249</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
         <v>320</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E17" t="s">
-        <v>243</v>
+        <v>161</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" t="s">
+        <v>341</v>
       </c>
       <c r="G17" t="s">
-        <v>248</v>
-      </c>
-      <c r="I17" s="11" t="str">
+        <v>339</v>
+      </c>
+      <c r="I17" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G17), G17)</f>
-        <v>2057-PH1-06-UA-ND</v>
+        <v>2057-USB-B-S-RA-WT-SPCC-ND</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -2288,83 +2301,82 @@
         <v>1</v>
       </c>
       <c r="L17" s="3">
-        <v>0.12</v>
+        <v>0.45</v>
       </c>
       <c r="M17" s="3">
         <f>J17*L17</f>
-        <v>0.12</v>
+        <v>0.45</v>
       </c>
       <c r="N17" t="s">
         <v>352</v>
       </c>
       <c r="O17" t="str">
         <f>_xlfn.CONCAT(N17, "-",C17)</f>
-        <v>MBP-J3</v>
+        <v>MBP-J2</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>340</v>
       </c>
       <c r="B18" t="s">
         <v>320</v>
       </c>
       <c r="C18" t="s">
-        <v>346</v>
+        <v>161</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" t="s">
-        <v>314</v>
+        <v>343</v>
       </c>
       <c r="G18" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I18" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G18), G18)</f>
-        <v>2057-PH2-12-UA-ND</v>
+        <v>102-4000-ND</v>
       </c>
       <c r="J18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <f>J18</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L18" s="3">
-        <v>0.18</v>
+        <v>0.75</v>
       </c>
       <c r="M18" s="3">
         <f>J18*L18</f>
-        <v>0.36</v>
+        <v>0.75</v>
       </c>
       <c r="N18" t="s">
         <v>352</v>
       </c>
       <c r="O18" t="str">
         <f>_xlfn.CONCAT(N18, "-",C18)</f>
-        <v>MBP-J4, J3</v>
+        <v>MBP-J2</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>249</v>
       </c>
       <c r="B19" t="s">
         <v>320</v>
       </c>
       <c r="C19" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" t="s">
-        <v>341</v>
+        <v>164</v>
+      </c>
+      <c r="E19" t="s">
+        <v>243</v>
       </c>
       <c r="G19" t="s">
-        <v>339</v>
-      </c>
-      <c r="I19" s="2" t="str">
+        <v>248</v>
+      </c>
+      <c r="I19" s="11" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G19), G19)</f>
-        <v>2057-USB-B-S-RA-WT-SPCC-ND</v>
+        <v>2057-PH1-06-UA-ND</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -2374,82 +2386,82 @@
         <v>1</v>
       </c>
       <c r="L19" s="3">
-        <v>0.45</v>
+        <v>0.12</v>
       </c>
       <c r="M19" s="3">
         <f>J19*L19</f>
-        <v>0.45</v>
-      </c>
-      <c r="N19" t="s">
-        <v>352</v>
+        <v>0.12</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>351</v>
       </c>
       <c r="O19" t="str">
         <f>_xlfn.CONCAT(N19, "-",C19)</f>
-        <v>MBP-J2</v>
+        <v>PSB-J3</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>250</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
         <v>320</v>
       </c>
       <c r="C20" t="s">
-        <v>258</v>
-      </c>
-      <c r="E20" t="s">
-        <v>243</v>
+        <v>346</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" t="s">
+        <v>314</v>
       </c>
       <c r="G20" t="s">
-        <v>251</v>
-      </c>
-      <c r="I20" s="11" t="str">
+        <v>344</v>
+      </c>
+      <c r="I20" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G20), G20)</f>
-        <v>S7039-ND</v>
+        <v>2057-PH2-12-UA-ND</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K20">
         <f>J20</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L20" s="3">
-        <v>0.53</v>
+        <v>0.18</v>
       </c>
       <c r="M20" s="3">
         <f>J20*L20</f>
-        <v>0.53</v>
+        <v>0.36</v>
       </c>
       <c r="N20" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="O20" t="str">
         <f>_xlfn.CONCAT(N20, "-",C20)</f>
-        <v>PSB-J5</v>
+        <v>MBP-J4, J3</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>340</v>
+        <v>250</v>
       </c>
       <c r="B21" t="s">
         <v>320</v>
       </c>
       <c r="C21" t="s">
-        <v>161</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" t="s">
-        <v>343</v>
+        <v>258</v>
+      </c>
+      <c r="E21" t="s">
+        <v>243</v>
       </c>
       <c r="G21" t="s">
-        <v>342</v>
-      </c>
-      <c r="I21" s="2" t="str">
+        <v>251</v>
+      </c>
+      <c r="I21" s="11" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G21), G21)</f>
-        <v>102-4000-ND</v>
+        <v>S7039-ND</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -2459,18 +2471,18 @@
         <v>1</v>
       </c>
       <c r="L21" s="3">
-        <v>0.75</v>
+        <v>0.53</v>
       </c>
       <c r="M21" s="3">
         <f>J21*L21</f>
-        <v>0.75</v>
+        <v>0.53</v>
       </c>
       <c r="N21" t="s">
         <v>352</v>
       </c>
       <c r="O21" t="str">
         <f>_xlfn.CONCAT(N21, "-",C21)</f>
-        <v>MBP-J2</v>
+        <v>MBP-J5</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2643,32 +2655,35 @@
         <v>0.84</v>
       </c>
       <c r="N25" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="O25" t="str">
         <f>_xlfn.CONCAT(N25, "-",C25)</f>
-        <v>PSB-NA</v>
+        <v>MBP-NA</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>226</v>
-      </c>
-      <c r="F26" t="s">
-        <v>355</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>74</v>
+        <v>220</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" t="s">
+        <v>63</v>
       </c>
       <c r="I26" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G26), G26)</f>
-        <v>336-5888-1-ND</v>
+        <v>ATMEGA328PB-AURCT-ND</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2678,42 +2693,39 @@
         <v>1</v>
       </c>
       <c r="L26" s="3">
-        <v>1.35</v>
+        <v>1.42</v>
       </c>
       <c r="M26" s="3">
         <f>J26*L26</f>
-        <v>1.35</v>
+        <v>1.42</v>
       </c>
       <c r="N26" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="O26" t="str">
         <f>_xlfn.CONCAT(N26, "-",C26)</f>
-        <v>PSB-U3</v>
+        <v>MBP-U1</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>220</v>
-      </c>
-      <c r="E27" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" t="s">
-        <v>85</v>
-      </c>
-      <c r="H27" t="s">
-        <v>63</v>
+        <v>226</v>
+      </c>
+      <c r="F27" t="s">
+        <v>355</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="I27" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G27), G27)</f>
-        <v>ATMEGA328PB-AURCT-ND</v>
+        <v>336-5888-1-ND</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2723,18 +2735,18 @@
         <v>1</v>
       </c>
       <c r="L27" s="3">
-        <v>1.42</v>
+        <v>1.35</v>
       </c>
       <c r="M27" s="3">
         <f>J27*L27</f>
-        <v>1.42</v>
-      </c>
-      <c r="N27" t="s">
-        <v>351</v>
+        <v>1.35</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>352</v>
       </c>
       <c r="O27" t="str">
         <f>_xlfn.CONCAT(N27, "-",C27)</f>
-        <v>PSB-U1</v>
+        <v>MBP-U3</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2773,89 +2785,89 @@
         <f>J28*L28</f>
         <v>0.36</v>
       </c>
-      <c r="N28" t="s">
-        <v>352</v>
+      <c r="N28" s="12" t="s">
+        <v>351</v>
       </c>
       <c r="O28" t="str">
         <f>_xlfn.CONCAT(N28, "-",C28)</f>
-        <v>MBP-U3</v>
+        <v>PSB-U3</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>357</v>
       </c>
       <c r="C29" t="s">
-        <v>265</v>
-      </c>
-      <c r="D29">
-        <v>10</v>
+        <v>271</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
       </c>
       <c r="E29" t="s">
         <v>100</v>
       </c>
       <c r="F29" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G29" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="I29" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G29), G29)</f>
-        <v>CR0805-JW-100ELFCT-ND</v>
+        <v>RMCF0805FT1K00CT-ND</v>
       </c>
       <c r="J29">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K29">
         <v>10</v>
       </c>
       <c r="L29" s="3">
-        <v>1.7999999999999999E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="M29" s="3">
         <f>J29*L29</f>
-        <v>0.14399999999999999</v>
+        <v>0.108</v>
       </c>
       <c r="N29" t="s">
         <v>352</v>
       </c>
       <c r="O29" t="str">
         <f>_xlfn.CONCAT(N29, "-",C29)</f>
-        <v>MBP-R29, R30, R31, R32, R33, R34, R35, R36</v>
+        <v>MBP-R1, R2, R21, R22</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>357</v>
       </c>
       <c r="C30" t="s">
-        <v>281</v>
-      </c>
-      <c r="D30" t="s">
-        <v>280</v>
+        <v>265</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
       </c>
       <c r="E30" t="s">
         <v>100</v>
       </c>
       <c r="F30" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="G30" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="I30" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G30), G30)</f>
-        <v>CR0805-JW-472ELFCT-ND</v>
+        <v>CR0805-JW-100ELFCT-ND</v>
       </c>
       <c r="J30">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K30">
         <v>10</v>
@@ -2865,347 +2877,347 @@
       </c>
       <c r="M30" s="3">
         <f>J30*L30</f>
-        <v>3.5999999999999997E-2</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="N30" t="s">
         <v>352</v>
       </c>
       <c r="O30" t="str">
         <f>_xlfn.CONCAT(N30, "-",C30)</f>
-        <v>MBP-R3, R4</v>
+        <v>MBP-R29, R30, R31, R32, R33, R34, R35, R36</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>313</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>357</v>
       </c>
       <c r="C31" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>280</v>
       </c>
       <c r="E31" t="s">
         <v>100</v>
       </c>
       <c r="F31" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G31" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="I31" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G31), G31)</f>
-        <v>RMCF0805FT1K00CT-ND</v>
+        <v>CR0805-JW-472ELFCT-ND</v>
       </c>
       <c r="J31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K31">
         <v>10</v>
       </c>
       <c r="L31" s="3">
-        <v>2.7E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M31" s="3">
         <f>J31*L31</f>
-        <v>0.108</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="N31" t="s">
         <v>352</v>
       </c>
       <c r="O31" t="str">
         <f>_xlfn.CONCAT(N31, "-",C31)</f>
-        <v>MBP-R1, R2, R21, R22</v>
+        <v>MBP-R3, R4</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>357</v>
       </c>
       <c r="C32" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" t="s">
-        <v>100</v>
+        <v>45</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="F32" t="s">
-        <v>322</v>
+        <v>240</v>
       </c>
       <c r="G32" t="s">
-        <v>321</v>
-      </c>
-      <c r="I32" s="2" t="str">
+        <v>239</v>
+      </c>
+      <c r="I32" s="11" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G32), G32)</f>
-        <v>RMCF0805FT30K1CT-ND</v>
+        <v>RMCF1206JT1K20CT-ND</v>
       </c>
       <c r="J32">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="K32">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L32" s="3">
-        <v>2.7E-2</v>
+        <v>0.1</v>
       </c>
       <c r="M32" s="3">
         <f>J32*L32</f>
-        <v>0.216</v>
+        <v>0.1</v>
       </c>
       <c r="N32" t="s">
         <v>351</v>
       </c>
       <c r="O32" t="str">
         <f>_xlfn.CONCAT(N32, "-",C32)</f>
-        <v>PSB-R5, R7, R11, R14, R15, R18, R19, R26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>PSB-R31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>357</v>
       </c>
       <c r="C33" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" t="s">
-        <v>100</v>
+        <v>44</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>324</v>
-      </c>
-      <c r="G33" t="s">
-        <v>323</v>
-      </c>
-      <c r="I33" s="2" t="str">
+        <v>238</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="I33" s="11" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G33), G33)</f>
-        <v>RMCF0805FT10K0CT-ND</v>
+        <v>RMCF1206JT390RCT-ND</v>
       </c>
       <c r="J33">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K33">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="L33" s="3">
-        <v>2.7E-2</v>
+        <v>0.1</v>
       </c>
       <c r="M33" s="3">
         <f>J33*L33</f>
-        <v>0.378</v>
+        <v>0.1</v>
       </c>
       <c r="N33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O33" t="str">
         <f>_xlfn.CONCAT(N33, "-",C33)</f>
-        <v>MBP-R6, R8, R10, R12, R13, R16, R17, R20, R24, R25, R27, R28, R37, R38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+        <v>PSB-R32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>357</v>
       </c>
       <c r="C34" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
-      </c>
-      <c r="E34" t="s">
-        <v>100</v>
+        <v>43</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="F34" t="s">
-        <v>325</v>
+        <v>236</v>
       </c>
       <c r="G34" t="s">
-        <v>326</v>
-      </c>
-      <c r="I34" s="2" t="str">
+        <v>235</v>
+      </c>
+      <c r="I34" s="11" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G34), G34)</f>
-        <v>RMCF0805FT15K0CT-ND</v>
+        <v>RMCF1206JT150RCT-ND</v>
       </c>
       <c r="J34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K34">
-        <v>10</v>
+        <f>J34</f>
+        <v>1</v>
       </c>
       <c r="L34" s="3">
-        <v>2.7E-2</v>
+        <v>0.1</v>
       </c>
       <c r="M34" s="3">
         <f>J34*L34</f>
-        <v>5.3999999999999999E-2</v>
+        <v>0.1</v>
       </c>
       <c r="N34" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O34" t="str">
         <f>_xlfn.CONCAT(N34, "-",C34)</f>
-        <v>MBP-R9, R23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+        <v>PSB-R33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>357</v>
       </c>
       <c r="C35" t="s">
-        <v>244</v>
+        <v>279</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>52</v>
+        <v>81</v>
+      </c>
+      <c r="E35" t="s">
+        <v>100</v>
       </c>
       <c r="F35" t="s">
-        <v>240</v>
+        <v>322</v>
       </c>
       <c r="G35" t="s">
-        <v>239</v>
-      </c>
-      <c r="I35" s="11" t="str">
+        <v>321</v>
+      </c>
+      <c r="I35" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G35), G35)</f>
-        <v>RMCF1206JT1K20CT-ND</v>
+        <v>RMCF0805FT30K1CT-ND</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K35">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L35" s="3">
-        <v>0.1</v>
+        <v>2.7E-2</v>
       </c>
       <c r="M35" s="3">
         <f>J35*L35</f>
-        <v>0.1</v>
+        <v>0.216</v>
       </c>
       <c r="N35" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="O35" t="str">
         <f>_xlfn.CONCAT(N35, "-",C35)</f>
-        <v>PSB-R31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+        <v>MBP-R5, R7, R11, R14, R15, R18, R19, R26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>357</v>
       </c>
       <c r="C36" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>52</v>
+        <v>80</v>
+      </c>
+      <c r="E36" t="s">
+        <v>100</v>
       </c>
       <c r="F36" t="s">
-        <v>238</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="I36" s="11" t="str">
+        <v>324</v>
+      </c>
+      <c r="G36" t="s">
+        <v>323</v>
+      </c>
+      <c r="I36" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G36), G36)</f>
-        <v>RMCF1206JT390RCT-ND</v>
+        <v>RMCF0805FT10K0CT-ND</v>
       </c>
       <c r="J36">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="K36">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="L36" s="3">
-        <v>0.1</v>
+        <v>2.7E-2</v>
       </c>
       <c r="M36" s="3">
         <f>J36*L36</f>
-        <v>0.1</v>
+        <v>0.378</v>
       </c>
       <c r="N36" t="s">
         <v>352</v>
       </c>
       <c r="O36" t="str">
         <f>_xlfn.CONCAT(N36, "-",C36)</f>
-        <v>MBP-R32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>MBP-R6, R8, R10, R12, R13, R16, R17, R20, R24, R25, R27, R28, R37, R38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>357</v>
       </c>
       <c r="C37" t="s">
-        <v>246</v>
+        <v>270</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>52</v>
+        <v>82</v>
+      </c>
+      <c r="E37" t="s">
+        <v>100</v>
       </c>
       <c r="F37" t="s">
-        <v>236</v>
+        <v>325</v>
       </c>
       <c r="G37" t="s">
-        <v>235</v>
-      </c>
-      <c r="I37" s="11" t="str">
+        <v>326</v>
+      </c>
+      <c r="I37" s="2" t="str">
         <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G37), G37)</f>
-        <v>RMCF1206JT150RCT-ND</v>
+        <v>RMCF0805FT15K0CT-ND</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K37">
-        <f>J37</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L37" s="3">
-        <v>0.1</v>
+        <v>2.7E-2</v>
       </c>
       <c r="M37" s="3">
         <f>J37*L37</f>
-        <v>0.1</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="N37" t="s">
         <v>352</v>
       </c>
       <c r="O37" t="str">
         <f>_xlfn.CONCAT(N37, "-",C37)</f>
-        <v>MBP-R33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+        <v>MBP-R9, R23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>234</v>
       </c>
@@ -3240,51 +3252,69 @@
         <v>0.43</v>
       </c>
       <c r="N38" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O38" t="str">
         <f>_xlfn.CONCAT(N38, "-",C38)</f>
-        <v>MBP-S3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+        <v>PSB-S3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>359</v>
+      </c>
+      <c r="P39" t="str">
+        <f>IF(ISNA(VLOOKUP(C39,'Main Board Additions'!$D$2:$D$33,1,FALSE)), "", "PSB")</f>
+        <v/>
+      </c>
+      <c r="Q39" t="str">
+        <f>IF(ISNA(VLOOKUP(C39,'MCU Board'!$C$2:$C$28,1,FALSE)), "", "MBP")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>359</v>
+      </c>
+      <c r="P40" t="str">
+        <f>IF(ISNA(VLOOKUP(C40,'Main Board Additions'!$D$2:$D$33,1,FALSE)), "", "PSB")</f>
+        <v/>
+      </c>
+      <c r="Q40" t="str">
+        <f>IF(ISNA(VLOOKUP(C40,'MCU Board'!$C$2:$C$28,1,FALSE)), "", "MBP")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L41" s="6" t="s">
         <v>350</v>
       </c>
       <c r="M41" s="6">
         <f>SUM(M2:M40)</f>
-        <v>19.465999999999994</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+        <v>19.465999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M45" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M32" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M38">
-      <sortCondition ref="B1:B32"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:O40" xr:uid="{30E9BFD1-6C3C-4845-8960-75181656E991}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O40">
     <sortCondition ref="C2:C40"/>
   </sortState>

</xml_diff>

<commit_message>
Added usb power. Switched optocouplers to active-high
</commit_message>
<xml_diff>
--- a/BOM_Initial.xlsx
+++ b/BOM_Initial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Gilliland\Desktop\All Projects\benchBuddy\benchBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D130C6E8-C747-4706-8779-EDBE9D2F5DC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08573845-5BB2-4FC9-BFF3-B9B40ECCA1EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PurchaseBOM" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="362">
   <si>
     <t>Usage</t>
   </si>
@@ -1123,6 +1123,9 @@
   </si>
   <si>
     <t>‎732-8074-1-ND‎</t>
+  </si>
+  <si>
+    <t>IC USB TO UART BRIDGE QFN24</t>
   </si>
 </sst>
 </file>
@@ -1235,13 +1238,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1271,6 +1267,13 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1552,7 +1555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1638,7 +1641,7 @@
         <v>333</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G2), G2)</f>
+        <f t="shared" ref="I2:I38" si="0">HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G2), G2)</f>
         <v>732-7816-1-ND</v>
       </c>
       <c r="J2">
@@ -1651,14 +1654,14 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="M2" s="3">
-        <f>J2*L2</f>
+        <f t="shared" ref="M2:M38" si="1">J2*L2</f>
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="N2" t="s">
         <v>352</v>
       </c>
       <c r="O2" t="str">
-        <f>_xlfn.CONCAT(N2, "-",C2)</f>
+        <f t="shared" ref="O2:O38" si="2">_xlfn.CONCAT(N2, "-",C2)</f>
         <v>MBP-C1, C2</v>
       </c>
     </row>
@@ -1685,7 +1688,7 @@
         <v>337</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G3), G3)</f>
+        <f t="shared" si="0"/>
         <v>732-12256-1-ND</v>
       </c>
       <c r="J3">
@@ -1698,14 +1701,14 @@
         <v>0.1</v>
       </c>
       <c r="M3" s="3">
-        <f>J3*L3</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="N3" t="s">
         <v>352</v>
       </c>
       <c r="O3" t="str">
-        <f>_xlfn.CONCAT(N3, "-",C3)</f>
+        <f t="shared" si="2"/>
         <v>MBP-C10, C11</v>
       </c>
     </row>
@@ -1729,7 +1732,7 @@
         <v>335</v>
       </c>
       <c r="I4" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G4), G4)</f>
+        <f t="shared" si="0"/>
         <v>1276-6471-1-ND</v>
       </c>
       <c r="J4">
@@ -1742,14 +1745,14 @@
         <v>4.7E-2</v>
       </c>
       <c r="M4" s="3">
-        <f>J4*L4</f>
+        <f t="shared" si="1"/>
         <v>0.188</v>
       </c>
       <c r="N4" t="s">
         <v>352</v>
       </c>
       <c r="O4" t="str">
-        <f>_xlfn.CONCAT(N4, "-",C4)</f>
+        <f t="shared" si="2"/>
         <v>MBP-C3, C5, C7, C9</v>
       </c>
     </row>
@@ -1773,7 +1776,7 @@
         <v>360</v>
       </c>
       <c r="I5" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G5), G5)</f>
+        <f t="shared" si="0"/>
         <v>‎732-8074-1-ND‎</v>
       </c>
       <c r="J5">
@@ -1786,14 +1789,14 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="M5" s="3">
-        <f>J5*L5</f>
+        <f t="shared" si="1"/>
         <v>0.10200000000000001</v>
       </c>
       <c r="N5" t="s">
         <v>352</v>
       </c>
       <c r="O5" t="str">
-        <f>_xlfn.CONCAT(N5, "-",C5)</f>
+        <f t="shared" si="2"/>
         <v>MBP-C4, C6, C8</v>
       </c>
     </row>
@@ -1817,7 +1820,7 @@
         <v>59</v>
       </c>
       <c r="I6" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G6), G6)</f>
+        <f t="shared" si="0"/>
         <v>1276-1007-1-ND</v>
       </c>
       <c r="J6">
@@ -1830,14 +1833,14 @@
         <v>0.04</v>
       </c>
       <c r="M6" s="3">
-        <f>J6*L6</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
       <c r="N6" t="s">
         <v>351</v>
       </c>
       <c r="O6" t="str">
-        <f>_xlfn.CONCAT(N6, "-",C6)</f>
+        <f t="shared" si="2"/>
         <v>PSB-C8, C11, C13</v>
       </c>
     </row>
@@ -1861,7 +1864,7 @@
         <v>336</v>
       </c>
       <c r="I7" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G7), G7)</f>
+        <f t="shared" si="0"/>
         <v>1276-6455-1-ND</v>
       </c>
       <c r="J7">
@@ -1874,14 +1877,14 @@
         <v>0.108</v>
       </c>
       <c r="M7" s="3">
-        <f>J7*L7</f>
+        <f t="shared" si="1"/>
         <v>0.432</v>
       </c>
       <c r="N7" t="s">
         <v>351</v>
       </c>
       <c r="O7" t="str">
-        <f>_xlfn.CONCAT(N7, "-",C7)</f>
+        <f t="shared" si="2"/>
         <v>PSB-C9, C10, C12, C14</v>
       </c>
     </row>
@@ -1902,7 +1905,7 @@
         <v>65</v>
       </c>
       <c r="I8" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G8), G8)</f>
+        <f t="shared" si="0"/>
         <v>576-1048-1-ND</v>
       </c>
       <c r="J8">
@@ -1916,14 +1919,14 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="M8" s="3">
-        <f>J8*L8</f>
+        <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
       <c r="N8" t="s">
         <v>352</v>
       </c>
       <c r="O8" t="str">
-        <f>_xlfn.CONCAT(N8, "-",C8)</f>
+        <f t="shared" si="2"/>
         <v>MBP-D1</v>
       </c>
     </row>
@@ -1947,7 +1950,7 @@
         <v>96</v>
       </c>
       <c r="I9" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G9), G9)</f>
+        <f t="shared" si="0"/>
         <v>507-1780-1-ND</v>
       </c>
       <c r="J9">
@@ -1960,14 +1963,14 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="M9" s="3">
-        <f>J9*L9</f>
+        <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="N9" t="s">
         <v>351</v>
       </c>
       <c r="O9" t="str">
-        <f>_xlfn.CONCAT(N9, "-",C9)</f>
+        <f t="shared" si="2"/>
         <v>PSB-F1</v>
       </c>
     </row>
@@ -1991,7 +1994,7 @@
         <v>41</v>
       </c>
       <c r="I10" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G10), G10)</f>
+        <f t="shared" si="0"/>
         <v>507-1761-1-ND</v>
       </c>
       <c r="J10">
@@ -2004,14 +2007,14 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="M10" s="3">
-        <f>J10*L10</f>
+        <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="N10" t="s">
         <v>351</v>
       </c>
       <c r="O10" t="str">
-        <f>_xlfn.CONCAT(N10, "-",C10)</f>
+        <f t="shared" si="2"/>
         <v>PSB-F2, F3</v>
       </c>
     </row>
@@ -2035,7 +2038,7 @@
         <v>37</v>
       </c>
       <c r="I11" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G11), G11)</f>
+        <f t="shared" si="0"/>
         <v>507-1763-1-ND</v>
       </c>
       <c r="J11">
@@ -2048,14 +2051,14 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="M11" s="3">
-        <f>J11*L11</f>
+        <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="N11" t="s">
         <v>351</v>
       </c>
       <c r="O11" t="str">
-        <f>_xlfn.CONCAT(N11, "-",C11)</f>
+        <f t="shared" si="2"/>
         <v>PSB-F2, F3</v>
       </c>
     </row>
@@ -2076,28 +2079,28 @@
         <v>69</v>
       </c>
       <c r="I12" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G12), G12)</f>
+        <f t="shared" si="0"/>
         <v>LM324DR2GOSCT-ND</v>
       </c>
       <c r="J12">
         <v>2</v>
       </c>
       <c r="K12">
-        <f>J12</f>
+        <f t="shared" ref="K12:K21" si="3">J12</f>
         <v>2</v>
       </c>
       <c r="L12" s="3">
         <v>0.35</v>
       </c>
       <c r="M12" s="3">
-        <f>J12*L12</f>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="N12" t="s">
         <v>352</v>
       </c>
       <c r="O12" t="str">
-        <f>_xlfn.CONCAT(N12, "-",C12)</f>
+        <f t="shared" si="2"/>
         <v>MBP-IC1, IC2</v>
       </c>
     </row>
@@ -2119,28 +2122,28 @@
         <v>347</v>
       </c>
       <c r="I13" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G13), G13)</f>
+        <f t="shared" si="0"/>
         <v>2057-PH2-06-UA-ND</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13">
-        <f>J13</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L13" s="3">
         <v>0.12</v>
       </c>
       <c r="M13" s="3">
-        <f>J13*L13</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
       <c r="N13" t="s">
         <v>352</v>
       </c>
       <c r="O13" t="str">
-        <f>_xlfn.CONCAT(N13, "-",C13)</f>
+        <f t="shared" si="2"/>
         <v>MBP-J1</v>
       </c>
     </row>
@@ -2162,28 +2165,28 @@
         <v>339</v>
       </c>
       <c r="I14" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G14), G14)</f>
+        <f t="shared" si="0"/>
         <v>2057-USB-B-S-RA-WT-SPCC-ND</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14">
-        <f>J14</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L14" s="3">
         <v>0.45</v>
       </c>
       <c r="M14" s="3">
-        <f>J14*L14</f>
+        <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
       <c r="N14" t="s">
         <v>352</v>
       </c>
       <c r="O14" t="str">
-        <f>_xlfn.CONCAT(N14, "-",C14)</f>
+        <f t="shared" si="2"/>
         <v>MBP-J2</v>
       </c>
     </row>
@@ -2205,28 +2208,28 @@
         <v>342</v>
       </c>
       <c r="I15" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G15), G15)</f>
+        <f t="shared" si="0"/>
         <v>102-4000-ND</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15">
-        <f>J15</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L15" s="3">
         <v>0.75</v>
       </c>
       <c r="M15" s="3">
-        <f>J15*L15</f>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="N15" t="s">
         <v>352</v>
       </c>
       <c r="O15" t="str">
-        <f>_xlfn.CONCAT(N15, "-",C15)</f>
+        <f t="shared" si="2"/>
         <v>MBP-J2</v>
       </c>
     </row>
@@ -2247,28 +2250,28 @@
         <v>248</v>
       </c>
       <c r="I16" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G16), G16)</f>
+        <f t="shared" si="0"/>
         <v>2057-PH1-06-UA-ND</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
       <c r="K16">
-        <f>J16</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L16" s="3">
         <v>0.12</v>
       </c>
       <c r="M16" s="3">
-        <f>J16*L16</f>
+        <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>351</v>
       </c>
       <c r="O16" t="str">
-        <f>_xlfn.CONCAT(N16, "-",C16)</f>
+        <f t="shared" si="2"/>
         <v>PSB-J3</v>
       </c>
     </row>
@@ -2290,28 +2293,28 @@
         <v>344</v>
       </c>
       <c r="I17" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G17), G17)</f>
+        <f t="shared" si="0"/>
         <v>2057-PH2-12-UA-ND</v>
       </c>
       <c r="J17">
         <v>2</v>
       </c>
       <c r="K17">
-        <f>J17</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L17" s="3">
         <v>0.18</v>
       </c>
       <c r="M17" s="3">
-        <f>J17*L17</f>
+        <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
       <c r="N17" t="s">
         <v>352</v>
       </c>
       <c r="O17" t="str">
-        <f>_xlfn.CONCAT(N17, "-",C17)</f>
+        <f t="shared" si="2"/>
         <v>MBP-J4, J3</v>
       </c>
     </row>
@@ -2332,28 +2335,28 @@
         <v>251</v>
       </c>
       <c r="I18" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G18), G18)</f>
+        <f t="shared" si="0"/>
         <v>S7039-ND</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
       <c r="K18">
-        <f>J18</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L18" s="3">
         <v>0.53</v>
       </c>
       <c r="M18" s="3">
-        <f>J18*L18</f>
+        <f t="shared" si="1"/>
         <v>0.53</v>
       </c>
       <c r="N18" t="s">
         <v>352</v>
       </c>
       <c r="O18" t="str">
-        <f>_xlfn.CONCAT(N18, "-",C18)</f>
+        <f t="shared" si="2"/>
         <v>MBP-J5</v>
       </c>
     </row>
@@ -2375,28 +2378,28 @@
         <v>315</v>
       </c>
       <c r="I19" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G19), G19)</f>
+        <f t="shared" si="0"/>
         <v>TLP185(GB-TPLSECT-ND</v>
       </c>
       <c r="J19">
         <v>2</v>
       </c>
       <c r="K19">
-        <f>J19</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L19" s="3">
         <v>0.42</v>
       </c>
       <c r="M19" s="3">
-        <f>J19*L19</f>
+        <f t="shared" si="1"/>
         <v>0.84</v>
       </c>
       <c r="N19" t="s">
         <v>352</v>
       </c>
       <c r="O19" t="str">
-        <f>_xlfn.CONCAT(N19, "-",C19)</f>
+        <f t="shared" si="2"/>
         <v>MBP-NA</v>
       </c>
     </row>
@@ -2420,28 +2423,28 @@
         <v>25</v>
       </c>
       <c r="I20" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G20), G20)</f>
+        <f t="shared" si="0"/>
         <v>102-5018-ND</v>
       </c>
       <c r="J20">
         <v>2</v>
       </c>
       <c r="K20">
-        <f>J20</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L20" s="3">
         <v>2.96</v>
       </c>
       <c r="M20" s="3">
-        <f>J20*L20</f>
+        <f t="shared" si="1"/>
         <v>5.92</v>
       </c>
       <c r="N20" t="s">
         <v>351</v>
       </c>
       <c r="O20" t="str">
-        <f>_xlfn.CONCAT(N20, "-",C20)</f>
+        <f t="shared" si="2"/>
         <v>PSB-PS1, PS2</v>
       </c>
     </row>
@@ -2465,28 +2468,28 @@
         <v>77</v>
       </c>
       <c r="I21" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G21), G21)</f>
+        <f t="shared" si="0"/>
         <v>887-2015-ND</v>
       </c>
       <c r="J21">
         <v>1</v>
       </c>
       <c r="K21">
-        <f>J21</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L21" s="3">
         <v>0.3</v>
       </c>
       <c r="M21" s="3">
-        <f>J21*L21</f>
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="N21" t="s">
         <v>352</v>
       </c>
       <c r="O21" t="str">
-        <f>_xlfn.CONCAT(N21, "-",C21)</f>
+        <f t="shared" si="2"/>
         <v>MBP-Q1</v>
       </c>
     </row>
@@ -2513,7 +2516,7 @@
         <v>327</v>
       </c>
       <c r="I22" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G22), G22)</f>
+        <f t="shared" si="0"/>
         <v>RMCF0805FT1K00CT-ND</v>
       </c>
       <c r="J22">
@@ -2526,14 +2529,14 @@
         <v>2.7E-2</v>
       </c>
       <c r="M22" s="3">
-        <f>J22*L22</f>
+        <f t="shared" si="1"/>
         <v>0.108</v>
       </c>
       <c r="N22" t="s">
         <v>352</v>
       </c>
       <c r="O22" t="str">
-        <f>_xlfn.CONCAT(N22, "-",C22)</f>
+        <f t="shared" si="2"/>
         <v>MBP-R1, R2, R21, R22</v>
       </c>
     </row>
@@ -2560,7 +2563,7 @@
         <v>331</v>
       </c>
       <c r="I23" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G23), G23)</f>
+        <f t="shared" si="0"/>
         <v>CR0805-JW-100ELFCT-ND</v>
       </c>
       <c r="J23">
@@ -2573,14 +2576,14 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="M23" s="3">
-        <f>J23*L23</f>
+        <f t="shared" si="1"/>
         <v>0.14399999999999999</v>
       </c>
       <c r="N23" t="s">
         <v>352</v>
       </c>
       <c r="O23" t="str">
-        <f>_xlfn.CONCAT(N23, "-",C23)</f>
+        <f t="shared" si="2"/>
         <v>MBP-R29, R30, R31, R32, R33, R34, R35, R36</v>
       </c>
     </row>
@@ -2607,7 +2610,7 @@
         <v>328</v>
       </c>
       <c r="I24" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G24), G24)</f>
+        <f t="shared" si="0"/>
         <v>CR0805-JW-472ELFCT-ND</v>
       </c>
       <c r="J24">
@@ -2620,14 +2623,14 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="M24" s="3">
-        <f>J24*L24</f>
+        <f t="shared" si="1"/>
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="N24" t="s">
         <v>352</v>
       </c>
       <c r="O24" t="str">
-        <f>_xlfn.CONCAT(N24, "-",C24)</f>
+        <f t="shared" si="2"/>
         <v>MBP-R3, R4</v>
       </c>
     </row>
@@ -2654,7 +2657,7 @@
         <v>239</v>
       </c>
       <c r="I25" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G25), G25)</f>
+        <f t="shared" si="0"/>
         <v>RMCF1206JT1K20CT-ND</v>
       </c>
       <c r="J25">
@@ -2667,14 +2670,14 @@
         <v>0.1</v>
       </c>
       <c r="M25" s="3">
-        <f>J25*L25</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="N25" t="s">
         <v>351</v>
       </c>
       <c r="O25" t="str">
-        <f>_xlfn.CONCAT(N25, "-",C25)</f>
+        <f t="shared" si="2"/>
         <v>PSB-R31</v>
       </c>
     </row>
@@ -2701,7 +2704,7 @@
         <v>237</v>
       </c>
       <c r="I26" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G26), G26)</f>
+        <f t="shared" si="0"/>
         <v>RMCF1206JT390RCT-ND</v>
       </c>
       <c r="J26">
@@ -2714,14 +2717,14 @@
         <v>0.1</v>
       </c>
       <c r="M26" s="3">
-        <f>J26*L26</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="N26" t="s">
         <v>351</v>
       </c>
       <c r="O26" t="str">
-        <f>_xlfn.CONCAT(N26, "-",C26)</f>
+        <f t="shared" si="2"/>
         <v>PSB-R32</v>
       </c>
     </row>
@@ -2748,7 +2751,7 @@
         <v>235</v>
       </c>
       <c r="I27" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G27), G27)</f>
+        <f t="shared" si="0"/>
         <v>RMCF1206JT150RCT-ND</v>
       </c>
       <c r="J27">
@@ -2762,14 +2765,14 @@
         <v>0.1</v>
       </c>
       <c r="M27" s="3">
-        <f>J27*L27</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="N27" t="s">
         <v>351</v>
       </c>
       <c r="O27" t="str">
-        <f>_xlfn.CONCAT(N27, "-",C27)</f>
+        <f t="shared" si="2"/>
         <v>PSB-R33</v>
       </c>
     </row>
@@ -2796,7 +2799,7 @@
         <v>321</v>
       </c>
       <c r="I28" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G28), G28)</f>
+        <f t="shared" si="0"/>
         <v>RMCF0805FT30K1CT-ND</v>
       </c>
       <c r="J28">
@@ -2809,14 +2812,14 @@
         <v>2.7E-2</v>
       </c>
       <c r="M28" s="3">
-        <f>J28*L28</f>
+        <f t="shared" si="1"/>
         <v>0.216</v>
       </c>
       <c r="N28" t="s">
         <v>352</v>
       </c>
       <c r="O28" t="str">
-        <f>_xlfn.CONCAT(N28, "-",C28)</f>
+        <f t="shared" si="2"/>
         <v>MBP-R5, R7, R11, R14, R15, R18, R19, R26</v>
       </c>
     </row>
@@ -2843,7 +2846,7 @@
         <v>323</v>
       </c>
       <c r="I29" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G29), G29)</f>
+        <f t="shared" si="0"/>
         <v>RMCF0805FT10K0CT-ND</v>
       </c>
       <c r="J29">
@@ -2856,14 +2859,14 @@
         <v>2.7E-2</v>
       </c>
       <c r="M29" s="3">
-        <f>J29*L29</f>
+        <f t="shared" si="1"/>
         <v>0.378</v>
       </c>
       <c r="N29" t="s">
         <v>352</v>
       </c>
       <c r="O29" t="str">
-        <f>_xlfn.CONCAT(N29, "-",C29)</f>
+        <f t="shared" si="2"/>
         <v>MBP-R6, R8, R10, R12, R13, R16, R17, R20, R24, R25, R27, R28, R37, R38</v>
       </c>
     </row>
@@ -2890,7 +2893,7 @@
         <v>326</v>
       </c>
       <c r="I30" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G30), G30)</f>
+        <f t="shared" si="0"/>
         <v>RMCF0805FT15K0CT-ND</v>
       </c>
       <c r="J30">
@@ -2903,14 +2906,14 @@
         <v>2.7E-2</v>
       </c>
       <c r="M30" s="3">
-        <f>J30*L30</f>
+        <f t="shared" si="1"/>
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="N30" t="s">
         <v>352</v>
       </c>
       <c r="O30" t="str">
-        <f>_xlfn.CONCAT(N30, "-",C30)</f>
+        <f t="shared" si="2"/>
         <v>MBP-R9, R23</v>
       </c>
     </row>
@@ -2934,7 +2937,7 @@
         <v>107</v>
       </c>
       <c r="I31" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G31), G31)</f>
+        <f t="shared" si="0"/>
         <v>CKN12220-1-ND</v>
       </c>
       <c r="J31">
@@ -2948,14 +2951,14 @@
         <v>0.1</v>
       </c>
       <c r="M31" s="3">
-        <f>J31*L31</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="N31" t="s">
         <v>352</v>
       </c>
       <c r="O31" t="str">
-        <f>_xlfn.CONCAT(N31, "-",C31)</f>
+        <f t="shared" si="2"/>
         <v>MBP-S1</v>
       </c>
     </row>
@@ -2976,7 +2979,7 @@
         <v>317</v>
       </c>
       <c r="I32" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G32), G32)</f>
+        <f t="shared" si="0"/>
         <v>401-2001-ND</v>
       </c>
       <c r="J32">
@@ -2990,14 +2993,14 @@
         <v>0.43</v>
       </c>
       <c r="M32" s="3">
-        <f>J32*L32</f>
+        <f t="shared" si="1"/>
         <v>0.43</v>
       </c>
       <c r="N32" t="s">
         <v>351</v>
       </c>
       <c r="O32" t="str">
-        <f>_xlfn.CONCAT(N32, "-",C32)</f>
+        <f t="shared" si="2"/>
         <v>PSB-S3</v>
       </c>
     </row>
@@ -3021,7 +3024,7 @@
         <v>63</v>
       </c>
       <c r="I33" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G33), G33)</f>
+        <f t="shared" si="0"/>
         <v>ATMEGA328PB-AURCT-ND</v>
       </c>
       <c r="J33">
@@ -3035,14 +3038,14 @@
         <v>1.42</v>
       </c>
       <c r="M33" s="3">
-        <f>J33*L33</f>
+        <f t="shared" si="1"/>
         <v>1.42</v>
       </c>
       <c r="N33" t="s">
         <v>352</v>
       </c>
       <c r="O33" t="str">
-        <f>_xlfn.CONCAT(N33, "-",C33)</f>
+        <f t="shared" si="2"/>
         <v>MBP-U1</v>
       </c>
     </row>
@@ -3066,7 +3069,7 @@
         <v>71</v>
       </c>
       <c r="I34" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G34), G34)</f>
+        <f t="shared" si="0"/>
         <v>AZ1117IH-5.0TRG1DICT-ND</v>
       </c>
       <c r="J34">
@@ -3079,14 +3082,14 @@
         <v>0.36</v>
       </c>
       <c r="M34" s="3">
-        <f>J34*L34</f>
+        <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
       <c r="N34" t="s">
         <v>352</v>
       </c>
       <c r="O34" t="str">
-        <f>_xlfn.CONCAT(N34, "-",C34)</f>
+        <f t="shared" si="2"/>
         <v>MBP-U2</v>
       </c>
     </row>
@@ -3110,7 +3113,7 @@
         <v>24</v>
       </c>
       <c r="I35" s="11" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G35), G35)</f>
+        <f t="shared" si="0"/>
         <v>AP2114HA-3.3TRG1DICT-ND</v>
       </c>
       <c r="J35">
@@ -3123,14 +3126,14 @@
         <v>0.36</v>
       </c>
       <c r="M35" s="3">
-        <f>J35*L35</f>
+        <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
       <c r="N35" s="12" t="s">
         <v>351</v>
       </c>
       <c r="O35" t="str">
-        <f>_xlfn.CONCAT(N35, "-",C35)</f>
+        <f t="shared" si="2"/>
         <v>PSB-U3</v>
       </c>
     </row>
@@ -3151,7 +3154,7 @@
         <v>74</v>
       </c>
       <c r="I36" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G36), G36)</f>
+        <f t="shared" si="0"/>
         <v>336-5888-1-ND</v>
       </c>
       <c r="J36">
@@ -3165,14 +3168,14 @@
         <v>1.35</v>
       </c>
       <c r="M36" s="3">
-        <f>J36*L36</f>
+        <f t="shared" si="1"/>
         <v>1.35</v>
       </c>
       <c r="N36" s="12" t="s">
         <v>352</v>
       </c>
       <c r="O36" t="str">
-        <f>_xlfn.CONCAT(N36, "-",C36)</f>
+        <f t="shared" si="2"/>
         <v>MBP-U3</v>
       </c>
     </row>
@@ -3190,7 +3193,7 @@
         <v>75</v>
       </c>
       <c r="I37" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G37), G37)</f>
+        <f t="shared" si="0"/>
         <v>1727-1582-1-ND</v>
       </c>
       <c r="J37">
@@ -3203,14 +3206,14 @@
         <v>0.31</v>
       </c>
       <c r="M37" s="3">
-        <f>J37*L37</f>
+        <f t="shared" si="1"/>
         <v>1.24</v>
       </c>
       <c r="N37" t="s">
         <v>352</v>
       </c>
       <c r="O37" t="str">
-        <f>_xlfn.CONCAT(N37, "-",C37)</f>
+        <f t="shared" si="2"/>
         <v>MBP-U4, U7, U8, U9</v>
       </c>
     </row>
@@ -3237,7 +3240,7 @@
         <v>115</v>
       </c>
       <c r="I38" s="2" t="str">
-        <f>HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",G38), G38)</f>
+        <f t="shared" si="0"/>
         <v>497-1192-1-ND</v>
       </c>
       <c r="J38">
@@ -3251,14 +3254,14 @@
         <v>0.4</v>
       </c>
       <c r="M38" s="3">
-        <f>J38*L38</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="N38" t="s">
         <v>352</v>
       </c>
       <c r="O38" t="str">
-        <f>_xlfn.CONCAT(N38, "-",C38)</f>
+        <f t="shared" si="2"/>
         <v>MBP-U6</v>
       </c>
     </row>
@@ -3327,7 +3330,7 @@
     <sortCondition ref="C2:C41"/>
   </sortState>
   <conditionalFormatting sqref="K2:K38">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>IF(K2 &lt;&gt; J2, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4158,10 +4161,10 @@
   </sheetData>
   <autoFilter ref="B1:O34" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="O2:O33">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="unchecked">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="unchecked">
       <formula>NOT(ISERROR(SEARCH("unchecked",O2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Need">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Need">
       <formula>NOT(ISERROR(SEARCH("Need",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4179,8 +4182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5039,6 +5042,9 @@
       <c r="C25" t="s">
         <v>226</v>
       </c>
+      <c r="F25" t="s">
+        <v>361</v>
+      </c>
       <c r="G25" s="10" t="s">
         <v>74</v>
       </c>
@@ -5303,10 +5309,10 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="N2:N34">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="unchecked">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="unchecked">
       <formula>NOT(ISERROR(SEARCH("unchecked",N2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Need">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Need">
       <formula>NOT(ISERROR(SEARCH("Need",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6623,7 +6629,7 @@
     <sortCondition ref="F2:F35"/>
   </sortState>
   <conditionalFormatting sqref="A2:A35">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="extra">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="extra">
       <formula>NOT(ISERROR(SEARCH("extra",A2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>